<commit_message>
Updated Lit Review (AH)
</commit_message>
<xml_diff>
--- a/Literature Review.xlsx
+++ b/Literature Review.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahook\Documents\Dissertation Research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86120A3E-F118-4CA2-B3CC-3BFCE7762E89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E56B6458-8D3B-4B90-A5B1-1B9A4B157603}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{61082C35-F1FB-43B8-8DDA-C44220570063}"/>
   </bookViews>
@@ -35,8 +35,40 @@
 </workbook>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata">
+  <metadataTypes count="1">
+    <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLRICHVALUE" count="2">
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="0"/>
+        </ext>
+      </extLst>
+    </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="1"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <valueMetadata count="2">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+    <bk>
+      <rc t="1" v="1"/>
+    </bk>
+  </valueMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t xml:space="preserve">Paper Title </t>
   </si>
@@ -237,11 +269,6 @@
     <t>Harrassment Categories (Labels)s</t>
   </si>
   <si>
-    <t>Verbal Harassment: This includes personal insults or hateful slurs directed towards individuals in the virtual environment.
-Physical Harassment: This encompasses simulated touching or grabbing, which can be particularly impactful due to the immersive nature of VR.
-Environmental Harassment: This type of harassment involves displaying graphic content on a shared screen within the VR space, affecting the environment experienced by users</t>
-  </si>
-  <si>
     <t>Not Public</t>
   </si>
   <si>
@@ -249,13 +276,259 @@
   </si>
   <si>
     <t>Schulenberg et al.</t>
+  </si>
+  <si>
+    <t>2023 CHI Conference on Human Factors in Computing Systems (CHI '23)</t>
+  </si>
+  <si>
+    <t>The paper focuses on the unique challenges of mitigating harassment in the immersive and embodied context of social virtual reality (VR). It highlights that current AI-based moderation systems face technical limitations in accurately detecting and addressing new forms of harassment specific to social VR, such as voice-based harassment. The study suggests the need for improved AI technologies and a re-envisioned approach to traditional moderation techniques to effectively combat the complex and nuanced nature of harassment in social VR environments</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">does not provide information about a publicly available dataset </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>related to harassment in social VR spaces. The content of the paper focuses on the findings from semi-structured interviews and the analysis of these interviews, rather than the compilation or mention of a dataset that is publicly accessible for further research.</t>
+    </r>
+  </si>
+  <si>
+    <t>Schulenberg, Kelsea, et al. "Towards Leveraging AI-based Moderation to Address Emergent Harassment in Social Virtual Reality." Proceedings of the 2023 CHI Conference on Human Factors in Computing Systems. 2023.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+The paper "The Experience of Social Touch in Multi-User Virtual Reality" presents a study on the emotional responses to virtual social touch in a two-user VR environment. It explores how different levels of intimacy in virtual touch affect emotions such as relaxation, happiness, anxiety, disgust, and fear. The study uses full-body tracked avatars and focuses on both the initiator and receiver of touch, highlighting the complex interplay of intimacy, touch direction, and participant gender on emotional responses. This research contributes to understanding social interactions in VR and their emotional impact, especially in the context of developing more immersive and socially meaningful VR applications</t>
+  </si>
+  <si>
+    <t>1. Groping
+2. Verbal Abuse
+3. Stalking
+4. Intimidation
+5. Physical Harassment (in a virtual context)</t>
+  </si>
+  <si>
+    <t>26th ACM Symposium on Virtual Reality Software and Technology (VRST '20)</t>
+  </si>
+  <si>
+    <t>Sykownik &amp; Masuch</t>
+  </si>
+  <si>
+    <t>The Experience of Social Touch in Multi-User Virtual Reality</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Low Intimacy Body:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Contacts: These include gestures like high-fives, fist-bumps, and shoulder taps. Participants were involved in both initiating and receiving these touches.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>High Intimacy Body Contacts</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: These are more personal touches, including caressing the arm, caressing the face, and hugging. Similar to low intimacy contacts, these also involved both initiating and receiving actions.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">User study is </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Not Public</t>
+    </r>
+  </si>
+  <si>
+    <t>Sykownik, Philipp, and Maic Masuch. "The experience of social touch in multi-user virtual reality." Proceedings of the 26th ACM Symposium on Virtual Reality Software and Technology. 2020.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Verbal Harassmen</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">t: This includes personal insults or hateful slurs directed towards individuals in the virtual environment.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Physical Harassment</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: This encompasses simulated touching or grabbing, which can be particularly impactful due to the immersive nature of VR.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Environmental Harassment</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: This type of harassment involves displaying graphic content on a shared screen within the VR space, affecting the environment experienced by users</t>
+    </r>
+  </si>
+  <si>
+    <t>ACM IVA 21</t>
+  </si>
+  <si>
+    <t>Sadeh-Sharvit, Shiri, et al. "Virtual reality in sexual harassment prevention: proof-of-concept study." Proceedings of the 21st ACM International Conference on Intelligent Virtual Agents. 2021.</t>
+  </si>
+  <si>
+    <t>Virtual Reality in Sexual Harassment Prevention: Proof-of-Concept Study</t>
+  </si>
+  <si>
+    <t>Sadeh-Sharvit et al.</t>
+  </si>
+  <si>
+    <t>The paper presents a novel virtual reality (VR) study focusing on sexual harassment prevention. Utilizing VR technology, the researchers created a simulated job interview scenario to explore individual responses to sexual harassment situations. This simulation included inappropriate comments, personal questions, and uncomfortable scenarios, designed to mimic real-life dynamics of workplace harassment. The study's technical contribution lies in its innovative use of VR as an immersive tool for understanding and training individuals to recognize and respond to sexual harassment. By analyzing participant responses and the physical and psychological impacts of these VR experiences, the study underscores VR's potential as a powerful medium for effective harassment prevention training.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Inappropriate Comments</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: The virtual interviewer makes comments about the participant's appearance, which are personal and unprofessional in the context of a job interview.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Personal Questions</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: Questions are asked that are too personal for a professional setting, crossing boundaries typically respected in a workplace.</t>
+    </r>
+  </si>
+  <si>
+    <t>No Dataset</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -284,6 +557,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="20"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -343,11 +624,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -365,6 +643,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -437,6 +721,75 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/richData/rdRichValueTypes.xml><?xml version="1.0" encoding="utf-8"?>
+<rvTypesInfo xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x">
+  <global>
+    <keyFlags>
+      <key name="_Self">
+        <flag name="ExcludeFromFile" value="1"/>
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_DisplayString">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Flags">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Format">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_SubLabel">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Attribution">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Icon">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_Display">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_CanonicalPropertyNames">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+      <key name="_ClassificationId">
+        <flag name="ExcludeFromCalcComparison" value="1"/>
+      </key>
+    </keyFlags>
+  </global>
+</rvTypesInfo>
+</file>
+
+<file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="2">
+  <rv s="0">
+    <v>0</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>1</v>
+    <v>5</v>
+  </rv>
+</rvData>
+</file>
+
+<file path=xl/richData/rdrichvaluestructure.xml><?xml version="1.0" encoding="utf-8"?>
+<rvStructures xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="1">
+  <s t="_localImage">
+    <k n="_rvRel:LocalImageIdentifier" t="i"/>
+    <k n="CalcOrigin" t="i"/>
+  </s>
+</rvStructures>
+</file>
+
+<file path=xl/richData/richValueRel.xml><?xml version="1.0" encoding="utf-8"?>
+<richValueRels xmlns="http://schemas.microsoft.com/office/spreadsheetml/2022/richvaluerel" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <rel r:id="rId1"/>
+  <rel r:id="rId2"/>
+</richValueRels>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -739,443 +1092,496 @@
   <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="33.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17.85546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="7.7109375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="35.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="35.7109375" style="2" customWidth="1"/>
-    <col min="7" max="7" width="33.42578125" style="2" customWidth="1"/>
-    <col min="8" max="9" width="33.140625" style="2" customWidth="1"/>
-    <col min="10" max="10" width="117" style="2" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="33.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="35.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="35.7109375" style="1" customWidth="1"/>
+    <col min="7" max="7" width="33.42578125" style="1" customWidth="1"/>
+    <col min="8" max="9" width="33.140625" style="1" customWidth="1"/>
+    <col min="10" max="10" width="117" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:10" ht="96.75" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="H1" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="361.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="2">
         <v>2019</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="E2" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="H2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I2" s="5" t="str">
+        <f>HYPERLINK("Papers To Read\VR Social\Done\0.pdf","View Paper")</f>
+        <v>View Paper</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="H2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I2" s="6" t="str">
-        <f>HYPERLINK("Papers To Read\VR Social\Done\3359202.pdf","View Paper")</f>
+      <c r="B3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="3">
+        <v>2023</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" s="6" t="str">
+        <f>HYPERLINK("Papers To Read\VR Social\done\1.pdf", "View Paper")</f>
         <v>View Paper</v>
       </c>
-      <c r="J2" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="99" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" s="4">
-        <v>2023</v>
-      </c>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="7" t="str">
-        <f>HYPERLINK("\Papers To Read\VR Social\0.pdf", "View Paper")</f>
+      <c r="J3" s="3"/>
+    </row>
+    <row r="4" spans="1:10" ht="315" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="2">
+        <v>2020</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I4" s="5" t="str">
+        <f>HYPERLINK("Papers To Read\VR Social\Done\2.pdf", "View Paper")</f>
         <v>View Paper</v>
       </c>
-      <c r="J3" s="4"/>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" s="3"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
+      <c r="J4" s="2" t="e" vm="1">
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="345" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="3">
+        <v>21</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="I5" s="6" t="str">
+        <f>HYPERLINK("Papers To Read\VR Social\Done\3.pdf", "View Paper")</f>
+        <v>View Paper</v>
+      </c>
+      <c r="J5" s="3" t="e" vm="2">
+        <v>#VALUE!</v>
+      </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="3"/>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
+      <c r="A7" s="3"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="3"/>
+      <c r="E7" s="3"/>
+      <c r="F7" s="3"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="3"/>
+      <c r="I7" s="3"/>
+      <c r="J7" s="3"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
-      <c r="B8" s="3"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+      <c r="E9" s="3"/>
+      <c r="F9" s="3"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="3"/>
+      <c r="I9" s="3"/>
+      <c r="J9" s="3"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="4"/>
-      <c r="B11" s="4"/>
-      <c r="C11" s="4"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
-      <c r="H11" s="4"/>
-      <c r="I11" s="4"/>
-      <c r="J11" s="4"/>
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="4"/>
-      <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
-      <c r="H13" s="4"/>
-      <c r="I13" s="4"/>
-      <c r="J13" s="4"/>
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="E13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
+      <c r="I13" s="3"/>
+      <c r="J13" s="3"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="4"/>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="4"/>
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="3"/>
+      <c r="I15" s="3"/>
+      <c r="J15" s="3"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" s="3"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" s="4"/>
-      <c r="B17" s="4"/>
-      <c r="C17" s="4"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
-      <c r="H17" s="4"/>
-      <c r="I17" s="4"/>
-      <c r="J17" s="4"/>
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" s="3"/>
-      <c r="B18" s="3"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" s="4"/>
-      <c r="B19" s="4"/>
-      <c r="C19" s="4"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
-      <c r="J19" s="4"/>
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" s="4"/>
-      <c r="B21" s="4"/>
-      <c r="C21" s="4"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="4"/>
-      <c r="I21" s="4"/>
-      <c r="J21" s="4"/>
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+      <c r="G21" s="3"/>
+      <c r="H21" s="3"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" s="3"/>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
-      <c r="J22" s="3"/>
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" s="4"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
-      <c r="H23" s="4"/>
-      <c r="I23" s="4"/>
-      <c r="J23" s="4"/>
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
+      <c r="H23" s="3"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" s="3"/>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
-      <c r="H24" s="3"/>
-      <c r="I24" s="3"/>
-      <c r="J24" s="3"/>
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
+      <c r="H24" s="2"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" s="4"/>
-      <c r="B25" s="4"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
-      <c r="H25" s="4"/>
-      <c r="I25" s="4"/>
-      <c r="J25" s="4"/>
+      <c r="A25" s="3"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="3"/>
+      <c r="J25" s="3"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" s="3"/>
-      <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
-      <c r="I26" s="3"/>
-      <c r="J26" s="3"/>
+      <c r="A26" s="2"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="2"/>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="4"/>
-      <c r="B27" s="4"/>
-      <c r="C27" s="4"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
-      <c r="H27" s="4"/>
-      <c r="I27" s="4"/>
-      <c r="J27" s="4"/>
+      <c r="A27" s="3"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
+      <c r="J27" s="3"/>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="3"/>
-      <c r="B28" s="3"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="3"/>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
-      <c r="H28" s="3"/>
-      <c r="I28" s="3"/>
-      <c r="J28" s="3"/>
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
+      <c r="H28" s="2"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="4"/>
-      <c r="B29" s="4"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="4"/>
-      <c r="H29" s="4"/>
-      <c r="I29" s="4"/>
-      <c r="J29" s="4"/>
+      <c r="A29" s="3"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="3"/>
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="3"/>
-      <c r="B30" s="3"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="3"/>
-      <c r="G30" s="3"/>
-      <c r="H30" s="3"/>
-      <c r="I30" s="3"/>
-      <c r="J30" s="3"/>
+      <c r="A30" s="2"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="4"/>
-      <c r="B31" s="4"/>
-      <c r="C31" s="4"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
-      <c r="G31" s="4"/>
-      <c r="H31" s="4"/>
-      <c r="I31" s="4"/>
-      <c r="J31" s="4"/>
+      <c r="A31" s="3"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="3"/>
+      <c r="J31" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Updated sheet 3 to show taxonomy structure
</commit_message>
<xml_diff>
--- a/Literature Review.xlsx
+++ b/Literature Review.xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahook\Documents\Dissertation Research\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E56B6458-8D3B-4B90-A5B1-1B9A4B157603}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACB2F238-AA8B-4618-8FE1-BBAFDEEA3C35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{61082C35-F1FB-43B8-8DDA-C44220570063}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{61082C35-F1FB-43B8-8DDA-C44220570063}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -68,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="64">
   <si>
     <t xml:space="preserve">Paper Title </t>
   </si>
@@ -523,12 +525,123 @@
   <si>
     <t>No Dataset</t>
   </si>
+  <si>
+    <t>Milestones and Deliverables</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Estimated Completion Date</t>
+  </si>
+  <si>
+    <t>Milestones</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">VR Data Generation 1:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>•</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Task 1.1: Design Virtual Reality (VR) scenes
+• Task 1.2: Select characters to represent victim and aggresor
+• Task 1.3: Develop data collection process in Unity (autonmous robot)
+</t>
+    </r>
+  </si>
+  <si>
+    <t>Complete</t>
+  </si>
+  <si>
+    <t>Deliverables</t>
+  </si>
+  <si>
+    <t xml:space="preserve">VR Data Geration 1:
+• Task 1.4: Define sexual harassment taxonomy for final scene generation
+• Task 1.5: Implement taxonomy design in VR
+• Task 1.6: Generate dataset
+Evaluate SOTA on VR content mod 2: 
+Task 2.1: Benchmark how well ViT and content moderation platforms work on the developed dataset 
+</t>
+  </si>
+  <si>
+    <t>VR Sexual Harassment Evaluation:
+Milestones:
+1.)	Virtual Reality scene developed in Unity.
+The scene developed in Unity requires various considerations on the downstream pipeline for graphical display. A High Definition Rendering Pipeline was chosen to support the hypothesis that a more “real” look will facilitate easier fine-tuning of transformer based architectures and illicit higher accuracy on publicly available content moderation tools such as Google API &amp; ChatGPT vision moderation.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A deep learning approach to early identification of suggested sexual harassment from videos </t>
+  </si>
+  <si>
+    <t>Shetye et al.</t>
+  </si>
+  <si>
+    <t>Sexual assault
+Sexual Harassment
+Sexual Violence</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/drive/folders/1kRt-MisnnVqurdlDY90XfMHH0l5GbMxK</t>
+  </si>
+  <si>
+    <t>Real World</t>
+  </si>
+  <si>
+    <t>Virtual Reality</t>
+  </si>
+  <si>
+    <t>Visual Detection (modality)</t>
+  </si>
+  <si>
+    <t>MultiModal Detection</t>
+  </si>
+  <si>
+    <t>Action</t>
+  </si>
+  <si>
+    <t>Example</t>
+  </si>
+  <si>
+    <t>Source</t>
+  </si>
+  <si>
+    <t>Groping</t>
+  </si>
+  <si>
+    <t>Context --&gt;</t>
+  </si>
+  <si>
+    <t>Context(Real or Virtual)</t>
+  </si>
+  <si>
+    <t>Context (Real or Virtual)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -569,8 +682,47 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -595,8 +747,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.749992370372631"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -619,12 +789,167 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -650,6 +975,87 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="17" fontId="0" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1091,9 +1497,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06363A6A-D6C6-4942-9E27-66ABED06023B}">
   <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K3" sqref="K3"/>
+      <selection pane="bottomLeft" activeCell="G5" sqref="A1:J6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1271,16 +1677,24 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
+    <row r="6" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>50</v>
+      </c>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
+      <c r="F6" s="2" t="s">
+        <v>51</v>
+      </c>
       <c r="G6" s="2"/>
       <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
+      <c r="I6" s="5" t="s">
+        <v>52</v>
+      </c>
       <c r="J6" s="2"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -1584,7 +1998,878 @@
       <c r="J31" s="3"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="I6" r:id="rId1" xr:uid="{797A9A28-2CD0-4703-A483-7F7A22BD6795}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25586C22-88E5-4F26-BCE0-B3D50BA791B0}">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView topLeftCell="B2" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.7109375" style="9" customWidth="1"/>
+    <col min="2" max="2" width="32.5703125" customWidth="1"/>
+    <col min="3" max="3" width="20.28515625" customWidth="1"/>
+    <col min="4" max="4" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="105" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="81.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="116.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" s="14">
+        <v>45292</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="153.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>47</v>
+      </c>
+      <c r="C3" s="12"/>
+      <c r="D3" s="14">
+        <v>45444</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+      <c r="F6" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2FC56F6-3100-436F-92DF-CF61F9722B34}">
+  <dimension ref="A1:Q48"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K27" sqref="K27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11" customWidth="1"/>
+    <col min="2" max="2" width="21.7109375" customWidth="1"/>
+    <col min="3" max="3" width="20.85546875" customWidth="1"/>
+    <col min="4" max="4" width="18.85546875" customWidth="1"/>
+    <col min="5" max="5" width="0.7109375" customWidth="1"/>
+    <col min="9" max="9" width="1" customWidth="1"/>
+    <col min="10" max="10" width="18.140625" customWidth="1"/>
+    <col min="11" max="11" width="27.28515625" customWidth="1"/>
+    <col min="12" max="12" width="28.85546875" customWidth="1"/>
+    <col min="13" max="13" width="0.42578125" customWidth="1"/>
+    <col min="14" max="14" width="14.28515625" customWidth="1"/>
+    <col min="15" max="15" width="27.140625" customWidth="1"/>
+    <col min="16" max="16" width="18.28515625" customWidth="1"/>
+    <col min="17" max="17" width="0.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" ht="40.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="44" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="36" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" s="37"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="36" t="s">
+        <v>54</v>
+      </c>
+      <c r="G1" s="37"/>
+      <c r="H1" s="38"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="36" t="s">
+        <v>55</v>
+      </c>
+      <c r="K1" s="37"/>
+      <c r="L1" s="38"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="36" t="s">
+        <v>56</v>
+      </c>
+      <c r="O1" s="37"/>
+      <c r="P1" s="38"/>
+      <c r="Q1" s="16"/>
+    </row>
+    <row r="2" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="45"/>
+      <c r="B2" s="39" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" s="40" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2" s="16"/>
+      <c r="F2" s="40" t="s">
+        <v>57</v>
+      </c>
+      <c r="G2" s="40" t="s">
+        <v>58</v>
+      </c>
+      <c r="H2" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="I2" s="16"/>
+      <c r="J2" s="40" t="s">
+        <v>57</v>
+      </c>
+      <c r="K2" s="40" t="s">
+        <v>62</v>
+      </c>
+      <c r="L2" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="M2" s="16"/>
+      <c r="N2" s="40" t="s">
+        <v>57</v>
+      </c>
+      <c r="O2" s="40" t="s">
+        <v>63</v>
+      </c>
+      <c r="P2" s="41" t="s">
+        <v>59</v>
+      </c>
+      <c r="Q2" s="16"/>
+    </row>
+    <row r="3" spans="1:17" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="45"/>
+      <c r="B3" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="28" t="s">
+        <v>60</v>
+      </c>
+      <c r="G3" s="3"/>
+      <c r="H3" s="29"/>
+      <c r="I3" s="30"/>
+      <c r="J3" s="28"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="29"/>
+      <c r="M3" s="30"/>
+      <c r="N3" s="28"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="29"/>
+      <c r="Q3" s="16"/>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A4" s="45"/>
+      <c r="B4" s="31"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="30"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="32"/>
+      <c r="I4" s="30"/>
+      <c r="J4" s="31"/>
+      <c r="K4" s="2"/>
+      <c r="L4" s="32"/>
+      <c r="M4" s="30"/>
+      <c r="N4" s="31"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="32"/>
+      <c r="Q4" s="16"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A5" s="45"/>
+      <c r="B5" s="28"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="29"/>
+      <c r="E5" s="30"/>
+      <c r="F5" s="28"/>
+      <c r="G5" s="3"/>
+      <c r="H5" s="29"/>
+      <c r="I5" s="30"/>
+      <c r="J5" s="28"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="29"/>
+      <c r="M5" s="30"/>
+      <c r="N5" s="28"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="29"/>
+      <c r="Q5" s="16"/>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A6" s="45"/>
+      <c r="B6" s="31"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="30"/>
+      <c r="F6" s="31"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="32"/>
+      <c r="I6" s="30"/>
+      <c r="J6" s="31"/>
+      <c r="K6" s="2"/>
+      <c r="L6" s="32"/>
+      <c r="M6" s="30"/>
+      <c r="N6" s="31"/>
+      <c r="O6" s="2"/>
+      <c r="P6" s="32"/>
+      <c r="Q6" s="16"/>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A7" s="45"/>
+      <c r="B7" s="28"/>
+      <c r="C7" s="3"/>
+      <c r="D7" s="29"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="3"/>
+      <c r="H7" s="29"/>
+      <c r="I7" s="30"/>
+      <c r="J7" s="28"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="29"/>
+      <c r="M7" s="30"/>
+      <c r="N7" s="28"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="29"/>
+      <c r="Q7" s="16"/>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A8" s="45"/>
+      <c r="B8" s="31"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="32"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="31"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="32"/>
+      <c r="I8" s="30"/>
+      <c r="J8" s="31"/>
+      <c r="K8" s="2"/>
+      <c r="L8" s="32"/>
+      <c r="M8" s="30"/>
+      <c r="N8" s="31"/>
+      <c r="O8" s="2"/>
+      <c r="P8" s="32"/>
+      <c r="Q8" s="16"/>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A9" s="45"/>
+      <c r="B9" s="28"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="29"/>
+      <c r="E9" s="30"/>
+      <c r="F9" s="28"/>
+      <c r="G9" s="3"/>
+      <c r="H9" s="29"/>
+      <c r="I9" s="30"/>
+      <c r="J9" s="28"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="29"/>
+      <c r="M9" s="30"/>
+      <c r="N9" s="28"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="29"/>
+      <c r="Q9" s="16"/>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A10" s="45"/>
+      <c r="B10" s="31"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="30"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="32"/>
+      <c r="I10" s="30"/>
+      <c r="J10" s="31"/>
+      <c r="K10" s="2"/>
+      <c r="L10" s="32"/>
+      <c r="M10" s="30"/>
+      <c r="N10" s="31"/>
+      <c r="O10" s="2"/>
+      <c r="P10" s="32"/>
+      <c r="Q10" s="16"/>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A11" s="45"/>
+      <c r="B11" s="28"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="30"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="29"/>
+      <c r="I11" s="30"/>
+      <c r="J11" s="28"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="29"/>
+      <c r="M11" s="30"/>
+      <c r="N11" s="28"/>
+      <c r="O11" s="3"/>
+      <c r="P11" s="29"/>
+      <c r="Q11" s="16"/>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A12" s="45"/>
+      <c r="B12" s="31"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="30"/>
+      <c r="F12" s="31"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="32"/>
+      <c r="I12" s="30"/>
+      <c r="J12" s="31"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="32"/>
+      <c r="M12" s="30"/>
+      <c r="N12" s="31"/>
+      <c r="O12" s="2"/>
+      <c r="P12" s="32"/>
+      <c r="Q12" s="16"/>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A13" s="45"/>
+      <c r="B13" s="28"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="29"/>
+      <c r="E13" s="30"/>
+      <c r="F13" s="28"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="29"/>
+      <c r="I13" s="30"/>
+      <c r="J13" s="28"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="29"/>
+      <c r="M13" s="30"/>
+      <c r="N13" s="28"/>
+      <c r="O13" s="3"/>
+      <c r="P13" s="29"/>
+      <c r="Q13" s="16"/>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A14" s="45"/>
+      <c r="B14" s="31"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="32"/>
+      <c r="E14" s="30"/>
+      <c r="F14" s="31"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="32"/>
+      <c r="I14" s="30"/>
+      <c r="J14" s="31"/>
+      <c r="K14" s="2"/>
+      <c r="L14" s="32"/>
+      <c r="M14" s="30"/>
+      <c r="N14" s="31"/>
+      <c r="O14" s="2"/>
+      <c r="P14" s="32"/>
+      <c r="Q14" s="16"/>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A15" s="45"/>
+      <c r="B15" s="28"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="29"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="28"/>
+      <c r="G15" s="3"/>
+      <c r="H15" s="29"/>
+      <c r="I15" s="30"/>
+      <c r="J15" s="28"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="29"/>
+      <c r="M15" s="30"/>
+      <c r="N15" s="28"/>
+      <c r="O15" s="3"/>
+      <c r="P15" s="29"/>
+      <c r="Q15" s="16"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A16" s="45"/>
+      <c r="B16" s="31"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="31"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="32"/>
+      <c r="I16" s="30"/>
+      <c r="J16" s="31"/>
+      <c r="K16" s="2"/>
+      <c r="L16" s="32"/>
+      <c r="M16" s="30"/>
+      <c r="N16" s="31"/>
+      <c r="O16" s="2"/>
+      <c r="P16" s="32"/>
+      <c r="Q16" s="16"/>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A17" s="45"/>
+      <c r="B17" s="28"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="29"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="28"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="29"/>
+      <c r="I17" s="30"/>
+      <c r="J17" s="28"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="29"/>
+      <c r="M17" s="30"/>
+      <c r="N17" s="28"/>
+      <c r="O17" s="3"/>
+      <c r="P17" s="29"/>
+      <c r="Q17" s="16"/>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A18" s="45"/>
+      <c r="B18" s="31"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="32"/>
+      <c r="E18" s="30"/>
+      <c r="F18" s="31"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="32"/>
+      <c r="I18" s="30"/>
+      <c r="J18" s="31"/>
+      <c r="K18" s="2"/>
+      <c r="L18" s="32"/>
+      <c r="M18" s="30"/>
+      <c r="N18" s="31"/>
+      <c r="O18" s="2"/>
+      <c r="P18" s="32"/>
+      <c r="Q18" s="16"/>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A19" s="45"/>
+      <c r="B19" s="28"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="29"/>
+      <c r="E19" s="30"/>
+      <c r="F19" s="28"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="29"/>
+      <c r="I19" s="30"/>
+      <c r="J19" s="28"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="29"/>
+      <c r="M19" s="30"/>
+      <c r="N19" s="28"/>
+      <c r="O19" s="3"/>
+      <c r="P19" s="29"/>
+      <c r="Q19" s="16"/>
+    </row>
+    <row r="20" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="45"/>
+      <c r="B20" s="33"/>
+      <c r="C20" s="34"/>
+      <c r="D20" s="35"/>
+      <c r="E20" s="30"/>
+      <c r="F20" s="33"/>
+      <c r="G20" s="34"/>
+      <c r="H20" s="35"/>
+      <c r="I20" s="30"/>
+      <c r="J20" s="33"/>
+      <c r="K20" s="34"/>
+      <c r="L20" s="35"/>
+      <c r="M20" s="30"/>
+      <c r="N20" s="33"/>
+      <c r="O20" s="34"/>
+      <c r="P20" s="35"/>
+      <c r="Q20" s="16"/>
+    </row>
+    <row r="21" spans="1:17" ht="2.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="42"/>
+      <c r="C21" s="26"/>
+      <c r="D21" s="43"/>
+      <c r="E21" s="16"/>
+      <c r="F21" s="16"/>
+      <c r="G21" s="16"/>
+      <c r="H21" s="16"/>
+      <c r="I21" s="16"/>
+      <c r="J21" s="16"/>
+      <c r="K21" s="16"/>
+      <c r="L21" s="16"/>
+      <c r="M21" s="16"/>
+      <c r="N21" s="16"/>
+      <c r="O21" s="16"/>
+      <c r="P21" s="16"/>
+      <c r="Q21" s="16"/>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B22" s="18"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="20"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="18"/>
+      <c r="G22" s="19"/>
+      <c r="H22" s="20"/>
+      <c r="I22" s="16"/>
+      <c r="J22" s="18"/>
+      <c r="K22" s="19"/>
+      <c r="L22" s="20"/>
+      <c r="M22" s="16"/>
+      <c r="N22" s="18"/>
+      <c r="O22" s="19"/>
+      <c r="P22" s="20"/>
+      <c r="Q22" s="16"/>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B23" s="21"/>
+      <c r="C23" s="17"/>
+      <c r="D23" s="22"/>
+      <c r="E23" s="16"/>
+      <c r="F23" s="21"/>
+      <c r="G23" s="17"/>
+      <c r="H23" s="22"/>
+      <c r="I23" s="16"/>
+      <c r="J23" s="21"/>
+      <c r="K23" s="17"/>
+      <c r="L23" s="22"/>
+      <c r="M23" s="16"/>
+      <c r="N23" s="21"/>
+      <c r="O23" s="17"/>
+      <c r="P23" s="22"/>
+      <c r="Q23" s="16"/>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B24" s="21"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="22"/>
+      <c r="E24" s="16"/>
+      <c r="F24" s="21"/>
+      <c r="G24" s="17"/>
+      <c r="H24" s="22"/>
+      <c r="I24" s="16"/>
+      <c r="J24" s="21"/>
+      <c r="K24" s="17"/>
+      <c r="L24" s="22"/>
+      <c r="M24" s="16"/>
+      <c r="N24" s="21"/>
+      <c r="O24" s="17"/>
+      <c r="P24" s="22"/>
+      <c r="Q24" s="16"/>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B25" s="21"/>
+      <c r="C25" s="17"/>
+      <c r="D25" s="22"/>
+      <c r="E25" s="16"/>
+      <c r="F25" s="21"/>
+      <c r="G25" s="17"/>
+      <c r="H25" s="22"/>
+      <c r="I25" s="16"/>
+      <c r="J25" s="21"/>
+      <c r="K25" s="17"/>
+      <c r="L25" s="22"/>
+      <c r="M25" s="16"/>
+      <c r="N25" s="21"/>
+      <c r="O25" s="17"/>
+      <c r="P25" s="22"/>
+      <c r="Q25" s="16"/>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B26" s="21"/>
+      <c r="C26" s="17"/>
+      <c r="D26" s="22"/>
+      <c r="E26" s="16"/>
+      <c r="F26" s="21"/>
+      <c r="G26" s="17"/>
+      <c r="H26" s="22"/>
+      <c r="I26" s="16"/>
+      <c r="J26" s="21"/>
+      <c r="K26" s="17"/>
+      <c r="L26" s="22"/>
+      <c r="M26" s="16"/>
+      <c r="N26" s="21"/>
+      <c r="O26" s="17"/>
+      <c r="P26" s="22"/>
+      <c r="Q26" s="16"/>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B27" s="21"/>
+      <c r="C27" s="17"/>
+      <c r="D27" s="22"/>
+      <c r="E27" s="16"/>
+      <c r="F27" s="21"/>
+      <c r="G27" s="17"/>
+      <c r="H27" s="22"/>
+      <c r="I27" s="16"/>
+      <c r="J27" s="21"/>
+      <c r="K27" s="17"/>
+      <c r="L27" s="22"/>
+      <c r="M27" s="16"/>
+      <c r="N27" s="21"/>
+      <c r="O27" s="17"/>
+      <c r="P27" s="22"/>
+      <c r="Q27" s="16"/>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B28" s="21"/>
+      <c r="C28" s="17"/>
+      <c r="D28" s="22"/>
+      <c r="E28" s="16"/>
+      <c r="F28" s="21"/>
+      <c r="G28" s="17"/>
+      <c r="H28" s="22"/>
+      <c r="I28" s="16"/>
+      <c r="J28" s="21"/>
+      <c r="K28" s="17"/>
+      <c r="L28" s="22"/>
+      <c r="M28" s="16"/>
+      <c r="N28" s="21"/>
+      <c r="O28" s="17"/>
+      <c r="P28" s="22"/>
+      <c r="Q28" s="16"/>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B29" s="21"/>
+      <c r="C29" s="17"/>
+      <c r="D29" s="22"/>
+      <c r="E29" s="16"/>
+      <c r="F29" s="21"/>
+      <c r="G29" s="17"/>
+      <c r="H29" s="22"/>
+      <c r="I29" s="16"/>
+      <c r="J29" s="21"/>
+      <c r="K29" s="17"/>
+      <c r="L29" s="22"/>
+      <c r="M29" s="16"/>
+      <c r="N29" s="21"/>
+      <c r="O29" s="17"/>
+      <c r="P29" s="22"/>
+      <c r="Q29" s="16"/>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B30" s="21"/>
+      <c r="C30" s="17"/>
+      <c r="D30" s="22"/>
+      <c r="E30" s="16"/>
+      <c r="F30" s="21"/>
+      <c r="G30" s="17"/>
+      <c r="H30" s="22"/>
+      <c r="I30" s="16"/>
+      <c r="J30" s="21"/>
+      <c r="K30" s="17"/>
+      <c r="L30" s="22"/>
+      <c r="M30" s="16"/>
+      <c r="N30" s="21"/>
+      <c r="O30" s="17"/>
+      <c r="P30" s="22"/>
+      <c r="Q30" s="16"/>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B31" s="21"/>
+      <c r="C31" s="17"/>
+      <c r="D31" s="22"/>
+      <c r="E31" s="16"/>
+      <c r="F31" s="21"/>
+      <c r="G31" s="17"/>
+      <c r="H31" s="22"/>
+      <c r="I31" s="16"/>
+      <c r="J31" s="21"/>
+      <c r="K31" s="17"/>
+      <c r="L31" s="22"/>
+      <c r="M31" s="16"/>
+      <c r="N31" s="21"/>
+      <c r="O31" s="17"/>
+      <c r="P31" s="22"/>
+      <c r="Q31" s="16"/>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B32" s="21"/>
+      <c r="C32" s="17"/>
+      <c r="D32" s="22"/>
+      <c r="E32" s="16"/>
+      <c r="F32" s="21"/>
+      <c r="G32" s="17"/>
+      <c r="H32" s="22"/>
+      <c r="I32" s="16"/>
+      <c r="J32" s="21"/>
+      <c r="K32" s="17"/>
+      <c r="L32" s="22"/>
+      <c r="M32" s="16"/>
+      <c r="N32" s="21"/>
+      <c r="O32" s="17"/>
+      <c r="P32" s="22"/>
+      <c r="Q32" s="16"/>
+    </row>
+    <row r="33" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B33" s="21"/>
+      <c r="C33" s="17"/>
+      <c r="D33" s="22"/>
+      <c r="E33" s="16"/>
+      <c r="F33" s="21"/>
+      <c r="G33" s="17"/>
+      <c r="H33" s="22"/>
+      <c r="I33" s="16"/>
+      <c r="J33" s="21"/>
+      <c r="K33" s="17"/>
+      <c r="L33" s="22"/>
+      <c r="M33" s="16"/>
+      <c r="N33" s="21"/>
+      <c r="O33" s="17"/>
+      <c r="P33" s="22"/>
+      <c r="Q33" s="16"/>
+    </row>
+    <row r="34" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="B34" s="21"/>
+      <c r="C34" s="17"/>
+      <c r="D34" s="22"/>
+      <c r="E34" s="16"/>
+      <c r="F34" s="21"/>
+      <c r="G34" s="17"/>
+      <c r="H34" s="22"/>
+      <c r="I34" s="16"/>
+      <c r="J34" s="21"/>
+      <c r="K34" s="17"/>
+      <c r="L34" s="22"/>
+      <c r="M34" s="16"/>
+      <c r="N34" s="21"/>
+      <c r="O34" s="17"/>
+      <c r="P34" s="22"/>
+      <c r="Q34" s="16"/>
+    </row>
+    <row r="35" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="23"/>
+      <c r="C35" s="24"/>
+      <c r="D35" s="25"/>
+      <c r="E35" s="16"/>
+      <c r="F35" s="21"/>
+      <c r="G35" s="17"/>
+      <c r="H35" s="22"/>
+      <c r="I35" s="16"/>
+      <c r="J35" s="21"/>
+      <c r="K35" s="17"/>
+      <c r="L35" s="22"/>
+      <c r="M35" s="16"/>
+      <c r="N35" s="21"/>
+      <c r="O35" s="17"/>
+      <c r="P35" s="22"/>
+      <c r="Q35" s="16"/>
+    </row>
+    <row r="36" spans="2:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B36" s="23"/>
+      <c r="C36" s="24"/>
+      <c r="D36" s="25"/>
+      <c r="E36" s="26"/>
+      <c r="F36" s="23"/>
+      <c r="G36" s="24"/>
+      <c r="H36" s="25"/>
+      <c r="I36" s="26"/>
+      <c r="J36" s="23"/>
+      <c r="K36" s="24"/>
+      <c r="L36" s="25"/>
+      <c r="M36" s="26"/>
+      <c r="N36" s="23"/>
+      <c r="O36" s="24"/>
+      <c r="P36" s="25"/>
+      <c r="Q36" s="26"/>
+    </row>
+    <row r="37" spans="2:17" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B37" s="27"/>
+      <c r="C37" s="27"/>
+      <c r="D37" s="27"/>
+      <c r="E37" s="27"/>
+      <c r="F37" s="27"/>
+      <c r="G37" s="27"/>
+      <c r="H37" s="27"/>
+      <c r="I37" s="27"/>
+      <c r="J37" s="27"/>
+      <c r="K37" s="27"/>
+      <c r="L37" s="27"/>
+      <c r="M37" s="27"/>
+      <c r="N37" s="27"/>
+      <c r="O37" s="27"/>
+      <c r="P37" s="27"/>
+      <c r="Q37" s="16"/>
+    </row>
+    <row r="38" spans="2:17" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="27"/>
+      <c r="C38" s="27"/>
+      <c r="D38" s="27"/>
+      <c r="E38" s="27"/>
+      <c r="F38" s="27"/>
+      <c r="G38" s="27"/>
+      <c r="H38" s="27"/>
+      <c r="I38" s="27"/>
+      <c r="J38" s="27"/>
+      <c r="K38" s="27"/>
+      <c r="L38" s="27"/>
+      <c r="M38" s="27"/>
+      <c r="N38" s="27"/>
+      <c r="O38" s="27"/>
+      <c r="P38" s="27"/>
+      <c r="Q38" s="16"/>
+    </row>
+    <row r="39" spans="2:17" ht="2.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="27"/>
+      <c r="C39" s="27"/>
+      <c r="D39" s="27"/>
+      <c r="E39" s="27"/>
+      <c r="F39" s="27"/>
+      <c r="G39" s="27"/>
+      <c r="H39" s="27"/>
+      <c r="I39" s="27"/>
+      <c r="J39" s="27"/>
+      <c r="K39" s="27"/>
+      <c r="L39" s="27"/>
+      <c r="M39" s="27"/>
+      <c r="N39" s="27"/>
+      <c r="O39" s="27"/>
+      <c r="P39" s="27"/>
+      <c r="Q39" s="16"/>
+    </row>
+    <row r="48" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="K48" s="17"/>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="B37:P39"/>
+    <mergeCell ref="B1:D1"/>
+    <mergeCell ref="F1:H1"/>
+    <mergeCell ref="J1:L1"/>
+    <mergeCell ref="N1:P1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated LitReview sheet 4
</commit_message>
<xml_diff>
--- a/Literature Review.xlsx
+++ b/Literature Review.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahook\Documents\Dissertation Research\LLM-VR-CyberHarassment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahook\Documents\Dissertation Research\Adam Work\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA04024A-7193-425F-B26F-767348347456}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74ACA083-FA9A-45A2-9585-FAB7D7139A44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{61082C35-F1FB-43B8-8DDA-C44220570063}"/>
   </bookViews>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="119">
   <si>
     <t xml:space="preserve">Paper Title </t>
   </si>
@@ -638,9 +638,6 @@
     <t>Context (Real or Virtual)</t>
   </si>
   <si>
-    <t>Doxxing</t>
-  </si>
-  <si>
     <t>Touching</t>
   </si>
   <si>
@@ -686,20 +683,132 @@
     <t>Sexual assault enters virtual reality</t>
   </si>
   <si>
-    <t>[1], [2]</t>
-  </si>
-  <si>
     <t>Reader Roundtable: “Virtual Rape” Claim Brings Belgian Police to Second Life</t>
   </si>
   <si>
     <t>[3]</t>
+  </si>
+  <si>
+    <t>✔</t>
+  </si>
+  <si>
+    <t>VW Groping</t>
+  </si>
+  <si>
+    <t>VW Rape</t>
+  </si>
+  <si>
+    <t>RW Rape/Harassment/Groping/Touching/Verbal  Abuse</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unsafe  and  Harassed  in Public  Spaces:  A NATIONAL STREET  HARASSMENT REPORT </t>
+  </si>
+  <si>
+    <t>Public Masturbation</t>
+  </si>
+  <si>
+    <t>Sexual Assault</t>
+  </si>
+  <si>
+    <t>Following/Stalking</t>
+  </si>
+  <si>
+    <t>Constant Pestering</t>
+  </si>
+  <si>
+    <t>Discriminatory Harassment</t>
+  </si>
+  <si>
+    <t>Unwanted Kissing</t>
+  </si>
+  <si>
+    <t>Hate Speech</t>
+  </si>
+  <si>
+    <t>Inappropraite avatar</t>
+  </si>
+  <si>
+    <t>My First Virtual Reality Groping</t>
+  </si>
+  <si>
+    <t>[1], [2],[5]</t>
+  </si>
+  <si>
+    <t>Inappropriate Sexual Behavior</t>
+  </si>
+  <si>
+    <t>[4],[6]</t>
+  </si>
+  <si>
+    <t>[4]</t>
+  </si>
+  <si>
+    <t>[7]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[8] </t>
+  </si>
+  <si>
+    <t>The prevalence and nature of sexual harassment and assault against women and girls on public transport: an international review</t>
+  </si>
+  <si>
+    <t>Grabbing and rubbing against someone (Isnt this Groping????)</t>
+  </si>
+  <si>
+    <t>SEXUAL ASSAULT</t>
+  </si>
+  <si>
+    <t>[9]</t>
+  </si>
+  <si>
+    <t>Discrimination, harassment, abuse, and bullying in the workplace: Contribution of workplace injustice to occupational health disparities</t>
+  </si>
+  <si>
+    <t>[10]</t>
+  </si>
+  <si>
+    <t>Virtual Reality Is Full of Assholes Who Sexually Harass Me. Here's Why I Keep Going Back</t>
+  </si>
+  <si>
+    <t>Audio-Based Hate Speech Detection for the Metaverse using CNN</t>
+  </si>
+  <si>
+    <t>[11]</t>
+  </si>
+  <si>
+    <t>[12]</t>
+  </si>
+  <si>
+    <t>Doxing</t>
+  </si>
+  <si>
+    <t>[13]</t>
+  </si>
+  <si>
+    <t>[14]</t>
+  </si>
+  <si>
+    <t>What Does Sexual Coercion Look Like?</t>
+  </si>
+  <si>
+    <t>Sexual Coercion</t>
+  </si>
+  <si>
+    <t>Parent and Kid Reviews on
+VRChat</t>
+  </si>
+  <si>
+    <t>Innappropriate Avatars</t>
+  </si>
+  <si>
+    <t>Grooming</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -779,8 +888,20 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="11">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -841,6 +962,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="20">
     <border>
@@ -1030,7 +1163,7 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
+      <bottom style="thin">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -1042,7 +1175,7 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="thin">
         <color indexed="64"/>
       </top>
       <bottom style="thin">
@@ -1060,21 +1193,6 @@
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -1082,15 +1200,26 @@
     </border>
     <border>
       <left/>
-      <right style="medium">
+      <right style="thin">
         <color indexed="64"/>
       </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -1098,7 +1227,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1191,6 +1320,21 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="9" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1203,71 +1347,81 @@
     <xf numFmtId="0" fontId="8" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="17" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="9" borderId="17" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="15" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="16" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="16" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="18" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="16" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1279,6 +1433,8 @@
   <colors>
     <mruColors>
       <color rgb="FFFF9F9F"/>
+      <color rgb="FFFF8B8B"/>
+      <color rgb="FFFF7D7D"/>
     </mruColors>
   </colors>
   <extLst>
@@ -2295,7 +2451,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F2FC56F6-3100-436F-92DF-CF61F9722B34}">
   <dimension ref="A1:Q39"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A22" sqref="A22:P35"/>
     </sheetView>
   </sheetViews>
@@ -2321,29 +2477,29 @@
       <c r="A1" s="38" t="s">
         <v>61</v>
       </c>
-      <c r="B1" s="41" t="s">
+      <c r="B1" s="46" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="42"/>
-      <c r="D1" s="43"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="48"/>
       <c r="E1" s="15"/>
-      <c r="F1" s="41" t="s">
+      <c r="F1" s="46" t="s">
         <v>54</v>
       </c>
-      <c r="G1" s="42"/>
-      <c r="H1" s="43"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="48"/>
       <c r="I1" s="16"/>
-      <c r="J1" s="41" t="s">
+      <c r="J1" s="46" t="s">
         <v>55</v>
       </c>
-      <c r="K1" s="42"/>
-      <c r="L1" s="43"/>
+      <c r="K1" s="47"/>
+      <c r="L1" s="48"/>
       <c r="M1" s="16"/>
-      <c r="N1" s="41" t="s">
+      <c r="N1" s="46" t="s">
         <v>56</v>
       </c>
-      <c r="O1" s="42"/>
-      <c r="P1" s="43"/>
+      <c r="O1" s="47"/>
+      <c r="P1" s="48"/>
       <c r="Q1" s="16"/>
     </row>
     <row r="2" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
@@ -2973,57 +3129,57 @@
       <c r="Q36" s="16"/>
     </row>
     <row r="37" spans="2:17" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="40"/>
-      <c r="C37" s="40"/>
-      <c r="D37" s="40"/>
-      <c r="E37" s="40"/>
-      <c r="F37" s="40"/>
-      <c r="G37" s="40"/>
-      <c r="H37" s="40"/>
-      <c r="I37" s="40"/>
-      <c r="J37" s="40"/>
-      <c r="K37" s="40"/>
-      <c r="L37" s="40"/>
-      <c r="M37" s="40"/>
-      <c r="N37" s="40"/>
-      <c r="O37" s="40"/>
-      <c r="P37" s="40"/>
+      <c r="B37" s="45"/>
+      <c r="C37" s="45"/>
+      <c r="D37" s="45"/>
+      <c r="E37" s="45"/>
+      <c r="F37" s="45"/>
+      <c r="G37" s="45"/>
+      <c r="H37" s="45"/>
+      <c r="I37" s="45"/>
+      <c r="J37" s="45"/>
+      <c r="K37" s="45"/>
+      <c r="L37" s="45"/>
+      <c r="M37" s="45"/>
+      <c r="N37" s="45"/>
+      <c r="O37" s="45"/>
+      <c r="P37" s="45"/>
       <c r="Q37" s="16"/>
     </row>
     <row r="38" spans="2:17" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="40"/>
-      <c r="C38" s="40"/>
-      <c r="D38" s="40"/>
-      <c r="E38" s="40"/>
-      <c r="F38" s="40"/>
-      <c r="G38" s="40"/>
-      <c r="H38" s="40"/>
-      <c r="I38" s="40"/>
-      <c r="J38" s="40"/>
-      <c r="K38" s="40"/>
-      <c r="L38" s="40"/>
-      <c r="M38" s="40"/>
-      <c r="N38" s="40"/>
-      <c r="O38" s="40"/>
-      <c r="P38" s="40"/>
+      <c r="B38" s="45"/>
+      <c r="C38" s="45"/>
+      <c r="D38" s="45"/>
+      <c r="E38" s="45"/>
+      <c r="F38" s="45"/>
+      <c r="G38" s="45"/>
+      <c r="H38" s="45"/>
+      <c r="I38" s="45"/>
+      <c r="J38" s="45"/>
+      <c r="K38" s="45"/>
+      <c r="L38" s="45"/>
+      <c r="M38" s="45"/>
+      <c r="N38" s="45"/>
+      <c r="O38" s="45"/>
+      <c r="P38" s="45"/>
       <c r="Q38" s="16"/>
     </row>
     <row r="39" spans="2:17" ht="2.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="40"/>
-      <c r="C39" s="40"/>
-      <c r="D39" s="40"/>
-      <c r="E39" s="40"/>
-      <c r="F39" s="40"/>
-      <c r="G39" s="40"/>
-      <c r="H39" s="40"/>
-      <c r="I39" s="40"/>
-      <c r="J39" s="40"/>
-      <c r="K39" s="40"/>
-      <c r="L39" s="40"/>
-      <c r="M39" s="40"/>
-      <c r="N39" s="40"/>
-      <c r="O39" s="40"/>
-      <c r="P39" s="40"/>
+      <c r="B39" s="45"/>
+      <c r="C39" s="45"/>
+      <c r="D39" s="45"/>
+      <c r="E39" s="45"/>
+      <c r="F39" s="45"/>
+      <c r="G39" s="45"/>
+      <c r="H39" s="45"/>
+      <c r="I39" s="45"/>
+      <c r="J39" s="45"/>
+      <c r="K39" s="45"/>
+      <c r="L39" s="45"/>
+      <c r="M39" s="45"/>
+      <c r="N39" s="45"/>
+      <c r="O39" s="45"/>
+      <c r="P39" s="45"/>
       <c r="Q39" s="16"/>
     </row>
   </sheetData>
@@ -3042,8 +3198,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7A2A574-CCE1-411A-AF42-0ACA90961AAE}">
   <dimension ref="A1:T95"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3051,79 +3207,89 @@
     <col min="1" max="1" width="19.140625" customWidth="1"/>
     <col min="2" max="2" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="27.140625" customWidth="1"/>
-    <col min="4" max="4" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" customWidth="1"/>
     <col min="5" max="5" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16.7109375" customWidth="1"/>
-    <col min="10" max="10" width="15.85546875" customWidth="1"/>
+    <col min="10" max="10" width="42.5703125" customWidth="1"/>
     <col min="11" max="11" width="46.7109375" customWidth="1"/>
     <col min="15" max="15" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="57" t="s">
         <v>57</v>
       </c>
-      <c r="B1" s="53" t="s">
+      <c r="B1" s="57" t="s">
+        <v>70</v>
+      </c>
+      <c r="C1" s="57" t="s">
         <v>71</v>
       </c>
-      <c r="C1" s="54" t="s">
+      <c r="D1" s="57" t="s">
+        <v>66</v>
+      </c>
+      <c r="E1" s="57" t="s">
+        <v>67</v>
+      </c>
+      <c r="F1" s="60" t="s">
         <v>72</v>
       </c>
-      <c r="D1" s="53" t="s">
-        <v>67</v>
-      </c>
-      <c r="E1" s="53" t="s">
-        <v>68</v>
-      </c>
-      <c r="F1" s="53" t="s">
+      <c r="G1" s="65" t="s">
         <v>73</v>
       </c>
-      <c r="G1" s="53" t="s">
+      <c r="H1" s="71"/>
+      <c r="I1" s="49" t="s">
         <v>74</v>
       </c>
-      <c r="I1" s="59" t="s">
+      <c r="J1" s="49" t="s">
+        <v>57</v>
+      </c>
+      <c r="K1" s="49" t="s">
         <v>75</v>
       </c>
-      <c r="J1" s="59" t="s">
-        <v>57</v>
-      </c>
-      <c r="K1" s="59" t="s">
+      <c r="L1" s="49" t="s">
+        <v>2</v>
+      </c>
+      <c r="M1" s="72" t="s">
         <v>76</v>
       </c>
-      <c r="L1" s="59" t="s">
-        <v>2</v>
-      </c>
-      <c r="M1" s="57" t="s">
-        <v>77</v>
-      </c>
     </row>
     <row r="2" spans="1:20" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="49" t="s">
+      <c r="A2" s="66" t="s">
         <v>60</v>
       </c>
-      <c r="B2" s="55"/>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
-      <c r="E2" s="56"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="65" t="s">
-        <v>80</v>
-      </c>
-      <c r="I2" s="60" t="str">
+      <c r="B2" s="74" t="s">
+        <v>81</v>
+      </c>
+      <c r="C2" s="74" t="s">
+        <v>81</v>
+      </c>
+      <c r="D2" s="74" t="s">
+        <v>81</v>
+      </c>
+      <c r="E2" s="69"/>
+      <c r="F2" s="62" t="s">
+        <v>98</v>
+      </c>
+      <c r="G2" s="52" t="s">
+        <v>95</v>
+      </c>
+      <c r="H2" s="71"/>
+      <c r="I2" s="41" t="str">
         <f>HYPERLINK("http://www.digra.org/wp-content/uploads/digital-library/DiGRA_2020_paper_272.pdf", "[1]")</f>
         <v>[1]</v>
       </c>
-      <c r="J2" s="61" t="s">
-        <v>60</v>
+      <c r="J2" s="42" t="s">
+        <v>82</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="L2" s="61">
+        <v>77</v>
+      </c>
+      <c r="L2" s="42">
         <v>2020</v>
       </c>
-      <c r="M2" s="1"/>
+      <c r="M2" s="73"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
@@ -3133,31 +3299,40 @@
       <c r="T2" s="1"/>
     </row>
     <row r="3" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="45" t="s">
-        <v>70</v>
-      </c>
-      <c r="B3" s="45"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="45"/>
-      <c r="E3" s="45"/>
-      <c r="F3" s="45"/>
-      <c r="G3" s="50" t="s">
-        <v>82</v>
-      </c>
-      <c r="I3" s="62" t="str">
+      <c r="A3" s="58" t="s">
+        <v>64</v>
+      </c>
+      <c r="B3" s="68" t="s">
+        <v>81</v>
+      </c>
+      <c r="C3" s="68" t="s">
+        <v>81</v>
+      </c>
+      <c r="D3" s="74" t="s">
+        <v>81</v>
+      </c>
+      <c r="E3" s="69"/>
+      <c r="F3" s="53" t="s">
+        <v>97</v>
+      </c>
+      <c r="G3" s="53" t="s">
+        <v>80</v>
+      </c>
+      <c r="H3" s="71"/>
+      <c r="I3" s="43" t="str">
         <f>HYPERLINK("https://theconversation.com/sexual-assault-enters-virtual-reality-67971", "[2]")</f>
         <v>[2]</v>
       </c>
-      <c r="J3" s="63" t="s">
-        <v>60</v>
+      <c r="J3" s="44" t="s">
+        <v>82</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="L3" s="58">
+        <v>78</v>
+      </c>
+      <c r="L3" s="40">
         <v>2016</v>
       </c>
-      <c r="M3" s="1"/>
+      <c r="M3" s="73"/>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
@@ -3167,29 +3342,40 @@
       <c r="T3" s="1"/>
     </row>
     <row r="4" spans="1:20" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="44" t="s">
+      <c r="A4" s="66" t="s">
         <v>65</v>
       </c>
-      <c r="B4" s="44"/>
-      <c r="C4" s="44"/>
-      <c r="D4" s="44"/>
-      <c r="E4" s="44"/>
-      <c r="F4" s="44"/>
-      <c r="G4" s="44"/>
-      <c r="I4" s="60" t="str">
+      <c r="B4" s="74" t="s">
+        <v>81</v>
+      </c>
+      <c r="C4" s="74" t="s">
+        <v>81</v>
+      </c>
+      <c r="D4" s="69"/>
+      <c r="E4" s="74" t="s">
+        <v>81</v>
+      </c>
+      <c r="F4" s="62" t="s">
+        <v>98</v>
+      </c>
+      <c r="G4" s="62" t="s">
+        <v>99</v>
+      </c>
+      <c r="H4" s="71"/>
+      <c r="I4" s="41" t="str">
         <f>HYPERLINK("https://virtuallyblind.com/2007/04/24/open-roundtable-allegations-of-virtual-rape-bring-belgian-police-to-second-life/", "[3]")</f>
         <v>[3]</v>
       </c>
-      <c r="J4" s="61" t="s">
-        <v>70</v>
+      <c r="J4" s="42" t="s">
+        <v>83</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="L4" s="61">
+        <v>79</v>
+      </c>
+      <c r="L4" s="42">
         <v>2007</v>
       </c>
-      <c r="M4" s="1"/>
+      <c r="M4" s="73"/>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
@@ -3198,21 +3384,39 @@
       <c r="S4" s="1"/>
       <c r="T4" s="1"/>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A5" s="46" t="s">
-        <v>66</v>
-      </c>
-      <c r="B5" s="46"/>
-      <c r="C5" s="46"/>
-      <c r="D5" s="46"/>
-      <c r="E5" s="45"/>
-      <c r="F5" s="45"/>
-      <c r="G5" s="45"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="58"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="58"/>
-      <c r="M5" s="1"/>
+    <row r="5" spans="1:20" ht="45" x14ac:dyDescent="0.25">
+      <c r="A5" s="58" t="s">
+        <v>68</v>
+      </c>
+      <c r="B5" s="68" t="s">
+        <v>81</v>
+      </c>
+      <c r="C5" s="68" t="s">
+        <v>81</v>
+      </c>
+      <c r="D5" s="68" t="s">
+        <v>81</v>
+      </c>
+      <c r="E5" s="69"/>
+      <c r="F5" s="61" t="s">
+        <v>98</v>
+      </c>
+      <c r="G5" s="54"/>
+      <c r="H5" s="71"/>
+      <c r="I5" s="50" t="str">
+        <f>HYPERLINK("https://drulibrary.uoregon.edu/sites/drulibrary2.uoregon.edu/files/rpds/entry/file_for_download/National_Street_Harassment_Report.pdf  ", "[4]")</f>
+        <v>[4]</v>
+      </c>
+      <c r="J5" s="40" t="s">
+        <v>84</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="L5" s="40">
+        <v>2014</v>
+      </c>
+      <c r="M5" s="73"/>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
@@ -3221,21 +3425,39 @@
       <c r="S5" s="1"/>
       <c r="T5" s="1"/>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A6" s="47" t="s">
+    <row r="6" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="66" t="s">
         <v>69</v>
       </c>
-      <c r="B6" s="47"/>
-      <c r="C6" s="51"/>
-      <c r="D6" s="47"/>
-      <c r="E6" s="47"/>
-      <c r="F6" s="47"/>
-      <c r="G6" s="47"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="61"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="61"/>
-      <c r="M6" s="1"/>
+      <c r="B6" s="74" t="s">
+        <v>81</v>
+      </c>
+      <c r="C6" s="74" t="s">
+        <v>81</v>
+      </c>
+      <c r="D6" s="69"/>
+      <c r="E6" s="74" t="s">
+        <v>81</v>
+      </c>
+      <c r="F6" s="62" t="s">
+        <v>98</v>
+      </c>
+      <c r="G6" s="55"/>
+      <c r="H6" s="71"/>
+      <c r="I6" s="51" t="str">
+        <f>HYPERLINK("https://medium.com/athena-talks/my-first-virtual-reality-sexual-assault-2330410b62ee  ", "[5]")</f>
+        <v>[5]</v>
+      </c>
+      <c r="J6" s="42" t="s">
+        <v>60</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="L6" s="42">
+        <v>2016</v>
+      </c>
+      <c r="M6" s="73"/>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
@@ -3244,21 +3466,40 @@
       <c r="S6" s="1"/>
       <c r="T6" s="1"/>
     </row>
-    <row r="7" spans="1:20" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="45" t="s">
+    <row r="7" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="58" t="s">
+        <v>86</v>
+      </c>
+      <c r="B7" s="68" t="s">
+        <v>81</v>
+      </c>
+      <c r="C7" s="68" t="s">
+        <v>81</v>
+      </c>
+      <c r="D7" s="68" t="s">
+        <v>81</v>
+      </c>
+      <c r="E7" s="69"/>
+      <c r="F7" s="61" t="str">
+        <f>HYPERLINK("https://drulibrary.uoregon.edu/sites/drulibrary2.uoregon.edu/files/rpds/entry/file_for_download/National_Street_Harassment_Report.pdf  ", "[4]")</f>
+        <v>[4]</v>
+      </c>
+      <c r="G7" s="53"/>
+      <c r="H7" s="71"/>
+      <c r="I7" s="50" t="str">
+        <f>HYPERLINK("https://journals.healio.com/doi/full/10.3928/0098-9134-19961101-07  ", "[6]")</f>
+        <v>[6]</v>
+      </c>
+      <c r="J7" s="40" t="s">
         <v>64</v>
       </c>
-      <c r="B7" s="48"/>
-      <c r="C7" s="48"/>
-      <c r="D7" s="52"/>
-      <c r="E7" s="52"/>
-      <c r="F7" s="52"/>
-      <c r="G7" s="64"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="58"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="58"/>
-      <c r="M7" s="1"/>
+      <c r="K7" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="L7" s="40">
+        <v>2013</v>
+      </c>
+      <c r="M7" s="73"/>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
@@ -3267,12 +3508,39 @@
       <c r="S7" s="1"/>
       <c r="T7" s="1"/>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="I8" s="1"/>
-      <c r="J8" s="1"/>
-      <c r="K8" s="1"/>
-      <c r="L8" s="1"/>
-      <c r="M8" s="1"/>
+    <row r="8" spans="1:20" ht="63" x14ac:dyDescent="0.25">
+      <c r="A8" s="66" t="s">
+        <v>102</v>
+      </c>
+      <c r="B8" s="74" t="s">
+        <v>81</v>
+      </c>
+      <c r="C8" s="74" t="s">
+        <v>81</v>
+      </c>
+      <c r="D8" s="74" t="s">
+        <v>81</v>
+      </c>
+      <c r="E8" s="69"/>
+      <c r="F8" s="62" t="s">
+        <v>100</v>
+      </c>
+      <c r="G8" s="67"/>
+      <c r="H8" s="71"/>
+      <c r="I8" s="51" t="str">
+        <f>HYPERLINK("https://dl.acm.org/doi/abs/10.1145/3359202?casa_token=0NUecOTYG_YAAAAA:KvTubl6e8UnX8572gKMhU3ZCVQD5PPTJlPIb7DozmmEI2DNB2on9cf2V2y-QS7ruccgIDan_Us-_2w%22  ", "[7]")</f>
+        <v>[7]</v>
+      </c>
+      <c r="J8" s="42" t="s">
+        <v>65</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="L8" s="42">
+        <v>2019</v>
+      </c>
+      <c r="M8" s="73"/>
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
@@ -3281,12 +3549,39 @@
       <c r="S8" s="1"/>
       <c r="T8" s="1"/>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
-      <c r="M9" s="1"/>
+    <row r="9" spans="1:20" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="58" t="s">
+        <v>87</v>
+      </c>
+      <c r="B9" s="68" t="s">
+        <v>81</v>
+      </c>
+      <c r="C9" s="68" t="s">
+        <v>81</v>
+      </c>
+      <c r="D9" s="69"/>
+      <c r="E9" s="68" t="s">
+        <v>81</v>
+      </c>
+      <c r="F9" s="61" t="s">
+        <v>104</v>
+      </c>
+      <c r="G9" s="63"/>
+      <c r="H9" s="71"/>
+      <c r="I9" s="50" t="str">
+        <f>HYPERLINK("https://www.emerald.com/insight/content/doi/10.1108/JCRPP-08-2016-0016/full/pdf?title=the-prevalence-and-nature-of-sexual-harassment-and-assault-against-women-and-girls-on-public-transport-an-international-review", "[8]")</f>
+        <v>[8]</v>
+      </c>
+      <c r="J9" s="40" t="s">
+        <v>88</v>
+      </c>
+      <c r="K9" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="L9" s="40">
+        <v>2016</v>
+      </c>
+      <c r="M9" s="73"/>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
@@ -3295,12 +3590,41 @@
       <c r="S9" s="1"/>
       <c r="T9" s="1"/>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="I10" s="1"/>
-      <c r="J10" s="1"/>
-      <c r="K10" s="1"/>
-      <c r="L10" s="1"/>
-      <c r="M10" s="1"/>
+    <row r="10" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10" s="66" t="s">
+        <v>88</v>
+      </c>
+      <c r="B10" s="74" t="s">
+        <v>81</v>
+      </c>
+      <c r="C10" s="74" t="s">
+        <v>81</v>
+      </c>
+      <c r="D10" s="75" t="s">
+        <v>81</v>
+      </c>
+      <c r="E10" s="74" t="s">
+        <v>81</v>
+      </c>
+      <c r="F10" s="62" t="s">
+        <v>100</v>
+      </c>
+      <c r="G10" s="67"/>
+      <c r="H10" s="71"/>
+      <c r="I10" s="51" t="str">
+        <f>HYPERLINK("https://www.sciencedirect.com/science/article/pii/S0733862705700912?ref=pdf_download&amp;fr=RR-2&amp;rr=86e94c45fdb26b52  ", "[9]")</f>
+        <v>[9]</v>
+      </c>
+      <c r="J10" s="42" t="s">
+        <v>87</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="L10" s="42">
+        <v>1999</v>
+      </c>
+      <c r="M10" s="73"/>
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
@@ -3309,12 +3633,37 @@
       <c r="S10" s="1"/>
       <c r="T10" s="1"/>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="I11" s="1"/>
-      <c r="J11" s="1"/>
-      <c r="K11" s="1"/>
-      <c r="L11" s="1"/>
-      <c r="M11" s="1"/>
+    <row r="11" spans="1:20" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="58" t="s">
+        <v>89</v>
+      </c>
+      <c r="B11" s="68" t="s">
+        <v>81</v>
+      </c>
+      <c r="C11" s="68" t="s">
+        <v>81</v>
+      </c>
+      <c r="D11" s="69"/>
+      <c r="E11" s="68" t="s">
+        <v>81</v>
+      </c>
+      <c r="F11" s="63"/>
+      <c r="G11" s="63"/>
+      <c r="H11" s="71"/>
+      <c r="I11" s="50" t="str">
+        <f>HYPERLINK("https://pubmed.ncbi.nlm.nih.gov/23813664/  ", "[10]")</f>
+        <v>[10]</v>
+      </c>
+      <c r="J11" s="40" t="s">
+        <v>90</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="L11" s="40">
+        <v>2013</v>
+      </c>
+      <c r="M11" s="73"/>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
@@ -3323,12 +3672,39 @@
       <c r="S11" s="1"/>
       <c r="T11" s="1"/>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
-      <c r="L12" s="1"/>
-      <c r="M12" s="1"/>
+    <row r="12" spans="1:20" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="66" t="s">
+        <v>90</v>
+      </c>
+      <c r="B12" s="74" t="s">
+        <v>81</v>
+      </c>
+      <c r="C12" s="74" t="s">
+        <v>81</v>
+      </c>
+      <c r="D12" s="69"/>
+      <c r="E12" s="74" t="s">
+        <v>81</v>
+      </c>
+      <c r="F12" s="62" t="s">
+        <v>106</v>
+      </c>
+      <c r="G12" s="67"/>
+      <c r="H12" s="71"/>
+      <c r="I12" s="51" t="str">
+        <f>HYPERLINK("https://www.mic.com/articles/144470/sexual-harassment-in-virtual-reality  ", "[11]")</f>
+        <v>[11]</v>
+      </c>
+      <c r="J12" s="42" t="s">
+        <v>91</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="L12" s="42">
+        <v>2016</v>
+      </c>
+      <c r="M12" s="73"/>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
@@ -3337,12 +3713,39 @@
       <c r="S12" s="1"/>
       <c r="T12" s="1"/>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="I13" s="1"/>
-      <c r="J13" s="1"/>
-      <c r="K13" s="1"/>
-      <c r="L13" s="1"/>
-      <c r="M13" s="1"/>
+    <row r="13" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="58" t="s">
+        <v>91</v>
+      </c>
+      <c r="B13" s="70" t="s">
+        <v>81</v>
+      </c>
+      <c r="C13" s="68" t="s">
+        <v>81</v>
+      </c>
+      <c r="D13" s="68" t="s">
+        <v>81</v>
+      </c>
+      <c r="E13" s="69"/>
+      <c r="F13" s="63"/>
+      <c r="G13" s="61" t="s">
+        <v>109</v>
+      </c>
+      <c r="H13" s="71"/>
+      <c r="I13" s="56" t="str">
+        <f>HYPERLINK("https://www.researchgate.net/publication/365877973_Audio-Based_Hate_Speech_Detection_for_the_Metaverse_using_CNN ", "[12]")</f>
+        <v>[12]</v>
+      </c>
+      <c r="J13" s="40" t="s">
+        <v>92</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="L13" s="40">
+        <v>2022</v>
+      </c>
+      <c r="M13" s="73"/>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
@@ -3351,12 +3754,39 @@
       <c r="S13" s="1"/>
       <c r="T13" s="1"/>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
-      <c r="L14" s="1"/>
-      <c r="M14" s="1"/>
+    <row r="14" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14" s="66" t="s">
+        <v>92</v>
+      </c>
+      <c r="B14" s="74" t="s">
+        <v>81</v>
+      </c>
+      <c r="C14" s="76" t="s">
+        <v>81</v>
+      </c>
+      <c r="D14" s="69"/>
+      <c r="E14" s="74" t="s">
+        <v>81</v>
+      </c>
+      <c r="F14" s="67"/>
+      <c r="G14" s="62" t="s">
+        <v>110</v>
+      </c>
+      <c r="H14" s="71"/>
+      <c r="I14" s="51" t="str">
+        <f>HYPERLINK("https://onlinelibrary.wiley.com/doi/epdf/10.1002/9781119429128.iegmc009 ", "[13]")</f>
+        <v>[13]</v>
+      </c>
+      <c r="J14" s="42" t="s">
+        <v>111</v>
+      </c>
+      <c r="K14" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="L14" s="42">
+        <v>2020</v>
+      </c>
+      <c r="M14" s="73"/>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
@@ -3365,12 +3795,37 @@
       <c r="S14" s="1"/>
       <c r="T14" s="1"/>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
-      <c r="K15" s="1"/>
-      <c r="L15" s="1"/>
-      <c r="M15" s="1"/>
+    <row r="15" spans="1:20" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="58" t="s">
+        <v>111</v>
+      </c>
+      <c r="B15" s="69"/>
+      <c r="C15" s="68" t="s">
+        <v>81</v>
+      </c>
+      <c r="D15" s="69"/>
+      <c r="E15" s="68" t="s">
+        <v>81</v>
+      </c>
+      <c r="F15" s="61" t="s">
+        <v>112</v>
+      </c>
+      <c r="G15" s="61"/>
+      <c r="H15" s="71"/>
+      <c r="I15" s="56" t="str">
+        <f>HYPERLINK("https://www.commonsensemedia.org/game-reviews/vrchat/user-reviews/adult#:~:text=There%20are%20a%20lot%20of%20adults%20running,saying%20the%20N%20word%20)%20run%20around.", "[14]")</f>
+        <v>[14]</v>
+      </c>
+      <c r="J15" s="40" t="s">
+        <v>117</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="L15" s="40">
+        <v>2024</v>
+      </c>
+      <c r="M15" s="73"/>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
@@ -3379,12 +3834,37 @@
       <c r="S15" s="1"/>
       <c r="T15" s="1"/>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-      <c r="K16" s="1"/>
-      <c r="L16" s="1"/>
-      <c r="M16" s="1"/>
+    <row r="16" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="66" t="s">
+        <v>93</v>
+      </c>
+      <c r="B16" s="69"/>
+      <c r="C16" s="74" t="s">
+        <v>81</v>
+      </c>
+      <c r="D16" s="74" t="s">
+        <v>81</v>
+      </c>
+      <c r="E16" s="69"/>
+      <c r="F16" s="67"/>
+      <c r="G16" s="62" t="s">
+        <v>113</v>
+      </c>
+      <c r="H16" s="71"/>
+      <c r="I16" s="51" t="str">
+        <f>HYPERLINK("https://www.healthline.com/health/sexual-coercion#defining-what-happened", "[15]")</f>
+        <v>[15]</v>
+      </c>
+      <c r="J16" s="42" t="s">
+        <v>115</v>
+      </c>
+      <c r="K16" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="L16" s="42">
+        <v>2020</v>
+      </c>
+      <c r="M16" s="73"/>
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
       <c r="P16" s="1"/>
@@ -3393,12 +3873,30 @@
       <c r="S16" s="1"/>
       <c r="T16" s="1"/>
     </row>
-    <row r="17" spans="9:20" x14ac:dyDescent="0.25">
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-      <c r="K17" s="1"/>
-      <c r="L17" s="1"/>
-      <c r="M17" s="1"/>
+    <row r="17" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="59" t="s">
+        <v>115</v>
+      </c>
+      <c r="B17" s="68" t="s">
+        <v>81</v>
+      </c>
+      <c r="C17" s="68" t="s">
+        <v>81</v>
+      </c>
+      <c r="D17" s="69"/>
+      <c r="E17" s="68" t="s">
+        <v>81</v>
+      </c>
+      <c r="F17" s="61">
+        <v>15</v>
+      </c>
+      <c r="G17" s="64"/>
+      <c r="H17" s="71"/>
+      <c r="I17" s="40"/>
+      <c r="J17" s="40"/>
+      <c r="K17" s="2"/>
+      <c r="L17" s="40"/>
+      <c r="M17" s="73"/>
       <c r="N17" s="1"/>
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
@@ -3407,12 +3905,30 @@
       <c r="S17" s="1"/>
       <c r="T17" s="1"/>
     </row>
-    <row r="18" spans="9:20" x14ac:dyDescent="0.25">
-      <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
-      <c r="K18" s="1"/>
-      <c r="L18" s="1"/>
-      <c r="M18" s="1"/>
+    <row r="18" spans="1:20" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="59" t="s">
+        <v>118</v>
+      </c>
+      <c r="B18" s="68" t="s">
+        <v>81</v>
+      </c>
+      <c r="C18" s="68" t="s">
+        <v>81</v>
+      </c>
+      <c r="D18" s="69"/>
+      <c r="E18" s="68" t="s">
+        <v>81</v>
+      </c>
+      <c r="F18" s="61">
+        <v>16</v>
+      </c>
+      <c r="G18" s="64"/>
+      <c r="H18" s="71"/>
+      <c r="I18" s="42"/>
+      <c r="J18" s="42"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="42"/>
+      <c r="M18" s="73"/>
       <c r="N18" s="1"/>
       <c r="O18" s="1"/>
       <c r="P18" s="1"/>
@@ -3421,12 +3937,20 @@
       <c r="S18" s="1"/>
       <c r="T18" s="1"/>
     </row>
-    <row r="19" spans="9:20" x14ac:dyDescent="0.25">
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
-      <c r="L19" s="1"/>
-      <c r="M19" s="1"/>
+    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A19" s="71"/>
+      <c r="B19" s="71"/>
+      <c r="C19" s="71"/>
+      <c r="D19" s="71"/>
+      <c r="E19" s="71"/>
+      <c r="F19" s="71"/>
+      <c r="G19" s="71"/>
+      <c r="H19" s="71"/>
+      <c r="I19" s="40"/>
+      <c r="J19" s="40"/>
+      <c r="K19" s="2"/>
+      <c r="L19" s="40"/>
+      <c r="M19" s="73"/>
       <c r="N19" s="1"/>
       <c r="O19" s="1"/>
       <c r="P19" s="1"/>
@@ -3435,12 +3959,20 @@
       <c r="S19" s="1"/>
       <c r="T19" s="1"/>
     </row>
-    <row r="20" spans="9:20" x14ac:dyDescent="0.25">
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
-      <c r="K20" s="1"/>
-      <c r="L20" s="1"/>
-      <c r="M20" s="1"/>
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A20" s="71"/>
+      <c r="B20" s="71"/>
+      <c r="C20" s="71"/>
+      <c r="D20" s="71"/>
+      <c r="E20" s="71"/>
+      <c r="F20" s="71"/>
+      <c r="G20" s="71"/>
+      <c r="H20" s="71"/>
+      <c r="I20" s="42"/>
+      <c r="J20" s="42"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="42"/>
+      <c r="M20" s="73"/>
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
@@ -3449,12 +3981,20 @@
       <c r="S20" s="1"/>
       <c r="T20" s="1"/>
     </row>
-    <row r="21" spans="9:20" x14ac:dyDescent="0.25">
-      <c r="I21" s="1"/>
-      <c r="J21" s="1"/>
-      <c r="K21" s="1"/>
-      <c r="L21" s="1"/>
-      <c r="M21" s="1"/>
+    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A21" s="71"/>
+      <c r="B21" s="71"/>
+      <c r="C21" s="71"/>
+      <c r="D21" s="71"/>
+      <c r="E21" s="71"/>
+      <c r="F21" s="71"/>
+      <c r="G21" s="71"/>
+      <c r="H21" s="71"/>
+      <c r="I21" s="40"/>
+      <c r="J21" s="40"/>
+      <c r="K21" s="2"/>
+      <c r="L21" s="40"/>
+      <c r="M21" s="73"/>
       <c r="N21" s="1"/>
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
@@ -3463,12 +4003,20 @@
       <c r="S21" s="1"/>
       <c r="T21" s="1"/>
     </row>
-    <row r="22" spans="9:20" x14ac:dyDescent="0.25">
-      <c r="I22" s="1"/>
-      <c r="J22" s="1"/>
-      <c r="K22" s="1"/>
-      <c r="L22" s="1"/>
-      <c r="M22" s="1"/>
+    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A22" s="71"/>
+      <c r="B22" s="71"/>
+      <c r="C22" s="71"/>
+      <c r="D22" s="71"/>
+      <c r="E22" s="71"/>
+      <c r="F22" s="71"/>
+      <c r="G22" s="71"/>
+      <c r="H22" s="71"/>
+      <c r="I22" s="42"/>
+      <c r="J22" s="42"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="42"/>
+      <c r="M22" s="73"/>
       <c r="N22" s="1"/>
       <c r="O22" s="1"/>
       <c r="P22" s="1"/>
@@ -3477,12 +4025,20 @@
       <c r="S22" s="1"/>
       <c r="T22" s="1"/>
     </row>
-    <row r="23" spans="9:20" x14ac:dyDescent="0.25">
-      <c r="I23" s="1"/>
-      <c r="J23" s="1"/>
-      <c r="K23" s="1"/>
-      <c r="L23" s="1"/>
-      <c r="M23" s="1"/>
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A23" s="71"/>
+      <c r="B23" s="71"/>
+      <c r="C23" s="71"/>
+      <c r="D23" s="71"/>
+      <c r="E23" s="71"/>
+      <c r="F23" s="71"/>
+      <c r="G23" s="71"/>
+      <c r="H23" s="71"/>
+      <c r="I23" s="40"/>
+      <c r="J23" s="40"/>
+      <c r="K23" s="2"/>
+      <c r="L23" s="40"/>
+      <c r="M23" s="73"/>
       <c r="N23" s="1"/>
       <c r="O23" s="1"/>
       <c r="P23" s="1"/>
@@ -3491,12 +4047,20 @@
       <c r="S23" s="1"/>
       <c r="T23" s="1"/>
     </row>
-    <row r="24" spans="9:20" x14ac:dyDescent="0.25">
-      <c r="I24" s="1"/>
-      <c r="J24" s="1"/>
-      <c r="K24" s="1"/>
-      <c r="L24" s="1"/>
-      <c r="M24" s="1"/>
+    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A24" s="71"/>
+      <c r="B24" s="71"/>
+      <c r="C24" s="71"/>
+      <c r="D24" s="71"/>
+      <c r="E24" s="71"/>
+      <c r="F24" s="71"/>
+      <c r="G24" s="71"/>
+      <c r="H24" s="71"/>
+      <c r="I24" s="42"/>
+      <c r="J24" s="42"/>
+      <c r="K24" s="3"/>
+      <c r="L24" s="42"/>
+      <c r="M24" s="73"/>
       <c r="N24" s="1"/>
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
@@ -3505,12 +4069,20 @@
       <c r="S24" s="1"/>
       <c r="T24" s="1"/>
     </row>
-    <row r="25" spans="9:20" x14ac:dyDescent="0.25">
-      <c r="I25" s="1"/>
-      <c r="J25" s="1"/>
-      <c r="K25" s="1"/>
-      <c r="L25" s="1"/>
-      <c r="M25" s="1"/>
+    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A25" s="71"/>
+      <c r="B25" s="71"/>
+      <c r="C25" s="71"/>
+      <c r="D25" s="71"/>
+      <c r="E25" s="71"/>
+      <c r="F25" s="71"/>
+      <c r="G25" s="71"/>
+      <c r="H25" s="71"/>
+      <c r="I25" s="40"/>
+      <c r="J25" s="40"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="40"/>
+      <c r="M25" s="73"/>
       <c r="N25" s="1"/>
       <c r="O25" s="1"/>
       <c r="P25" s="1"/>
@@ -3519,12 +4091,20 @@
       <c r="S25" s="1"/>
       <c r="T25" s="1"/>
     </row>
-    <row r="26" spans="9:20" x14ac:dyDescent="0.25">
-      <c r="I26" s="1"/>
-      <c r="J26" s="1"/>
-      <c r="K26" s="1"/>
-      <c r="L26" s="1"/>
-      <c r="M26" s="1"/>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A26" s="71"/>
+      <c r="B26" s="71"/>
+      <c r="C26" s="71"/>
+      <c r="D26" s="71"/>
+      <c r="E26" s="71"/>
+      <c r="F26" s="71"/>
+      <c r="G26" s="71"/>
+      <c r="H26" s="71"/>
+      <c r="I26" s="42"/>
+      <c r="J26" s="42"/>
+      <c r="K26" s="3"/>
+      <c r="L26" s="42"/>
+      <c r="M26" s="73"/>
       <c r="N26" s="1"/>
       <c r="O26" s="1"/>
       <c r="P26" s="1"/>
@@ -3533,12 +4113,20 @@
       <c r="S26" s="1"/>
       <c r="T26" s="1"/>
     </row>
-    <row r="27" spans="9:20" x14ac:dyDescent="0.25">
-      <c r="I27" s="1"/>
-      <c r="J27" s="1"/>
-      <c r="K27" s="1"/>
-      <c r="L27" s="1"/>
-      <c r="M27" s="1"/>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A27" s="71"/>
+      <c r="B27" s="71"/>
+      <c r="C27" s="71"/>
+      <c r="D27" s="71"/>
+      <c r="E27" s="71"/>
+      <c r="F27" s="71"/>
+      <c r="G27" s="71"/>
+      <c r="H27" s="71"/>
+      <c r="I27" s="40"/>
+      <c r="J27" s="40"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="40"/>
+      <c r="M27" s="73"/>
       <c r="N27" s="1"/>
       <c r="O27" s="1"/>
       <c r="P27" s="1"/>
@@ -3547,12 +4135,20 @@
       <c r="S27" s="1"/>
       <c r="T27" s="1"/>
     </row>
-    <row r="28" spans="9:20" x14ac:dyDescent="0.25">
-      <c r="I28" s="1"/>
-      <c r="J28" s="1"/>
-      <c r="K28" s="1"/>
-      <c r="L28" s="1"/>
-      <c r="M28" s="1"/>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+      <c r="A28" s="71"/>
+      <c r="B28" s="71"/>
+      <c r="C28" s="71"/>
+      <c r="D28" s="71"/>
+      <c r="E28" s="71"/>
+      <c r="F28" s="71"/>
+      <c r="G28" s="71"/>
+      <c r="H28" s="71"/>
+      <c r="I28" s="42"/>
+      <c r="J28" s="42"/>
+      <c r="K28" s="3"/>
+      <c r="L28" s="42"/>
+      <c r="M28" s="73"/>
       <c r="N28" s="1"/>
       <c r="O28" s="1"/>
       <c r="P28" s="1"/>
@@ -3561,7 +4157,7 @@
       <c r="S28" s="1"/>
       <c r="T28" s="1"/>
     </row>
-    <row r="29" spans="9:20" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="I29" s="1"/>
       <c r="J29" s="1"/>
       <c r="K29" s="1"/>
@@ -3575,7 +4171,7 @@
       <c r="S29" s="1"/>
       <c r="T29" s="1"/>
     </row>
-    <row r="30" spans="9:20" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.25">
       <c r="I30" s="1"/>
       <c r="J30" s="1"/>
       <c r="K30" s="1"/>
@@ -3589,7 +4185,7 @@
       <c r="S30" s="1"/>
       <c r="T30" s="1"/>
     </row>
-    <row r="31" spans="9:20" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.25">
       <c r="I31" s="1"/>
       <c r="J31" s="1"/>
       <c r="K31" s="1"/>
@@ -3603,7 +4199,7 @@
       <c r="S31" s="1"/>
       <c r="T31" s="1"/>
     </row>
-    <row r="32" spans="9:20" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="I32" s="1"/>
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>

</xml_diff>

<commit_message>
Updated Taxonomy and Grounded Theory
</commit_message>
<xml_diff>
--- a/Literature Review.xlsx
+++ b/Literature Review.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahook\Documents\Dissertation Research\Adam Work\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31D53CA9-D7D2-4CC4-8A4F-1770211B8FD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4974011-D492-45A5-B698-788E30A81220}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{61082C35-F1FB-43B8-8DDA-C44220570063}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{61082C35-F1FB-43B8-8DDA-C44220570063}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
   <metadataTypes count="1">
     <metadataType name="XLRICHVALUE" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1"/>
   </metadataTypes>
-  <futureMetadata name="XLRICHVALUE" count="2">
+  <futureMetadata name="XLRICHVALUE" count="3">
     <bk>
       <extLst>
         <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
@@ -58,20 +58,30 @@
         </ext>
       </extLst>
     </bk>
+    <bk>
+      <extLst>
+        <ext uri="{3e2802c4-a4d2-4d8b-9148-e3be6c30e623}">
+          <xlrd:rvb i="2"/>
+        </ext>
+      </extLst>
+    </bk>
   </futureMetadata>
-  <valueMetadata count="2">
+  <valueMetadata count="3">
     <bk>
       <rc t="1" v="0"/>
     </bk>
     <bk>
       <rc t="1" v="1"/>
     </bk>
+    <bk>
+      <rc t="1" v="2"/>
+    </bk>
   </valueMetadata>
 </metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="130">
   <si>
     <t xml:space="preserve">Paper Title </t>
   </si>
@@ -695,9 +705,6 @@
     <t>VW Groping</t>
   </si>
   <si>
-    <t>VW Rape</t>
-  </si>
-  <si>
     <t>RW Rape/Harassment/Groping/Touching/Verbal  Abuse</t>
   </si>
   <si>
@@ -729,9 +736,6 @@
   </si>
   <si>
     <t>My First Virtual Reality Groping</t>
-  </si>
-  <si>
-    <t>[1], [2],[5]</t>
   </si>
   <si>
     <t>Inappropriate Sexual Behavior</t>
@@ -802,13 +806,55 @@
   </si>
   <si>
     <t>Grooming</t>
+  </si>
+  <si>
+    <t>Touching/VW Rape</t>
+  </si>
+  <si>
+    <t>[15]</t>
+  </si>
+  <si>
+    <t>[1],[2],[5]</t>
+  </si>
+  <si>
+    <t>Term</t>
+  </si>
+  <si>
+    <t>Definition</t>
+  </si>
+  <si>
+    <t>Tea Bagging</t>
+  </si>
+  <si>
+    <t>a largely accepted (though often unpleasant) behaviour seen most frequently in competitive first-person shooter games whereby one player crouches repeatedly over the head of another player lying on the ground in mimicry of a sexual act, usually to humiliate or assert victory over that player</t>
+  </si>
+  <si>
+    <t>[1]</t>
+  </si>
+  <si>
+    <t>Perhaps there could be three tiers of interaction:
+1.) Sexual Harassment
+2.) Sexual Assualt
+3.) Rape</t>
+  </si>
+  <si>
+    <t xml:space="preserve">From ‘Silly’ to ‘Scumbag’: Reddit Discussion of a Case of Groping in a Virtual Reality Game </t>
+  </si>
+  <si>
+    <t>Groping (RW)</t>
+  </si>
+  <si>
+    <t>Groping (VW)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[1] Find </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -899,6 +945,13 @@
       <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="13">
@@ -1158,7 +1211,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1285,18 +1338,6 @@
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1326,8 +1367,32 @@
     <xf numFmtId="0" fontId="11" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1450,13 +1515,17 @@
 </file>
 
 <file path=xl/richData/rdrichvalue.xml><?xml version="1.0" encoding="utf-8"?>
-<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="2">
+<rvData xmlns="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" count="3">
   <rv s="0">
     <v>0</v>
     <v>5</v>
   </rv>
   <rv s="0">
     <v>1</v>
+    <v>5</v>
+  </rv>
+  <rv s="0">
+    <v>2</v>
     <v>5</v>
   </rv>
 </rvData>
@@ -1475,6 +1544,7 @@
 <richValueRels xmlns="http://schemas.microsoft.com/office/spreadsheetml/2022/richvaluerel" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <rel r:id="rId1"/>
   <rel r:id="rId2"/>
+  <rel r:id="rId3"/>
 </richValueRels>
 </file>
 
@@ -1775,11 +1845,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06363A6A-D6C6-4942-9E27-66ABED06023B}">
-  <dimension ref="A1:J31"/>
+  <dimension ref="A1:K31"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G5" sqref="A1:J6"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1792,10 +1862,11 @@
     <col min="7" max="7" width="33.42578125" style="1" customWidth="1"/>
     <col min="8" max="9" width="33.140625" style="1" customWidth="1"/>
     <col min="10" max="10" width="117" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="1"/>
+    <col min="11" max="11" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="96.75" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:11" ht="96.75" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -1827,7 +1898,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="361.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="361.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>6</v>
       </c>
@@ -1860,7 +1931,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>17</v>
       </c>
@@ -1891,7 +1962,7 @@
       </c>
       <c r="J3" s="3"/>
     </row>
-    <row r="4" spans="1:10" ht="315" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="315" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>27</v>
       </c>
@@ -1924,7 +1995,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="345" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="345" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>34</v>
       </c>
@@ -1957,7 +2028,7 @@
         <v>#VALUE!</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>49</v>
       </c>
@@ -1977,8 +2048,10 @@
       </c>
       <c r="J6" s="2"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="3"/>
+    <row r="7" spans="1:11" ht="180.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>126</v>
+      </c>
       <c r="B7" s="3"/>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
@@ -1987,9 +2060,14 @@
       <c r="G7" s="3"/>
       <c r="H7" s="3"/>
       <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J7" s="2" t="e" vm="3">
+        <v>#VALUE!</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
@@ -1999,9 +2077,8 @@
       <c r="G8" s="2"/>
       <c r="H8" s="2"/>
       <c r="I8" s="2"/>
-      <c r="J8" s="2"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="3"/>
       <c r="B9" s="3"/>
       <c r="C9" s="3"/>
@@ -2013,7 +2090,7 @@
       <c r="I9" s="3"/>
       <c r="J9" s="3"/>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
@@ -2025,7 +2102,7 @@
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -2037,7 +2114,7 @@
       <c r="I11" s="3"/>
       <c r="J11" s="3"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="2"/>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
@@ -2049,7 +2126,7 @@
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -2061,7 +2138,7 @@
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -2073,7 +2150,7 @@
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="3"/>
       <c r="B15" s="3"/>
       <c r="C15" s="3"/>
@@ -2085,7 +2162,7 @@
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
@@ -2383,29 +2460,29 @@
       <c r="A1" s="38" t="s">
         <v>61</v>
       </c>
-      <c r="B1" s="53" t="s">
+      <c r="B1" s="67" t="s">
         <v>53</v>
       </c>
-      <c r="C1" s="54"/>
-      <c r="D1" s="55"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="69"/>
       <c r="E1" s="15"/>
-      <c r="F1" s="53" t="s">
+      <c r="F1" s="67" t="s">
         <v>54</v>
       </c>
-      <c r="G1" s="54"/>
-      <c r="H1" s="55"/>
+      <c r="G1" s="68"/>
+      <c r="H1" s="69"/>
       <c r="I1" s="16"/>
-      <c r="J1" s="53" t="s">
+      <c r="J1" s="67" t="s">
         <v>55</v>
       </c>
-      <c r="K1" s="54"/>
-      <c r="L1" s="55"/>
+      <c r="K1" s="68"/>
+      <c r="L1" s="69"/>
       <c r="M1" s="16"/>
-      <c r="N1" s="53" t="s">
+      <c r="N1" s="67" t="s">
         <v>56</v>
       </c>
-      <c r="O1" s="54"/>
-      <c r="P1" s="55"/>
+      <c r="O1" s="68"/>
+      <c r="P1" s="69"/>
       <c r="Q1" s="16"/>
     </row>
     <row r="2" spans="1:17" ht="15.75" x14ac:dyDescent="0.25">
@@ -3035,57 +3112,57 @@
       <c r="Q36" s="16"/>
     </row>
     <row r="37" spans="2:17" ht="5.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B37" s="52"/>
-      <c r="C37" s="52"/>
-      <c r="D37" s="52"/>
-      <c r="E37" s="52"/>
-      <c r="F37" s="52"/>
-      <c r="G37" s="52"/>
-      <c r="H37" s="52"/>
-      <c r="I37" s="52"/>
-      <c r="J37" s="52"/>
-      <c r="K37" s="52"/>
-      <c r="L37" s="52"/>
-      <c r="M37" s="52"/>
-      <c r="N37" s="52"/>
-      <c r="O37" s="52"/>
-      <c r="P37" s="52"/>
+      <c r="B37" s="66"/>
+      <c r="C37" s="66"/>
+      <c r="D37" s="66"/>
+      <c r="E37" s="66"/>
+      <c r="F37" s="66"/>
+      <c r="G37" s="66"/>
+      <c r="H37" s="66"/>
+      <c r="I37" s="66"/>
+      <c r="J37" s="66"/>
+      <c r="K37" s="66"/>
+      <c r="L37" s="66"/>
+      <c r="M37" s="66"/>
+      <c r="N37" s="66"/>
+      <c r="O37" s="66"/>
+      <c r="P37" s="66"/>
       <c r="Q37" s="16"/>
     </row>
     <row r="38" spans="2:17" ht="4.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="52"/>
-      <c r="C38" s="52"/>
-      <c r="D38" s="52"/>
-      <c r="E38" s="52"/>
-      <c r="F38" s="52"/>
-      <c r="G38" s="52"/>
-      <c r="H38" s="52"/>
-      <c r="I38" s="52"/>
-      <c r="J38" s="52"/>
-      <c r="K38" s="52"/>
-      <c r="L38" s="52"/>
-      <c r="M38" s="52"/>
-      <c r="N38" s="52"/>
-      <c r="O38" s="52"/>
-      <c r="P38" s="52"/>
+      <c r="B38" s="66"/>
+      <c r="C38" s="66"/>
+      <c r="D38" s="66"/>
+      <c r="E38" s="66"/>
+      <c r="F38" s="66"/>
+      <c r="G38" s="66"/>
+      <c r="H38" s="66"/>
+      <c r="I38" s="66"/>
+      <c r="J38" s="66"/>
+      <c r="K38" s="66"/>
+      <c r="L38" s="66"/>
+      <c r="M38" s="66"/>
+      <c r="N38" s="66"/>
+      <c r="O38" s="66"/>
+      <c r="P38" s="66"/>
       <c r="Q38" s="16"/>
     </row>
     <row r="39" spans="2:17" ht="2.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="52"/>
-      <c r="C39" s="52"/>
-      <c r="D39" s="52"/>
-      <c r="E39" s="52"/>
-      <c r="F39" s="52"/>
-      <c r="G39" s="52"/>
-      <c r="H39" s="52"/>
-      <c r="I39" s="52"/>
-      <c r="J39" s="52"/>
-      <c r="K39" s="52"/>
-      <c r="L39" s="52"/>
-      <c r="M39" s="52"/>
-      <c r="N39" s="52"/>
-      <c r="O39" s="52"/>
-      <c r="P39" s="52"/>
+      <c r="B39" s="66"/>
+      <c r="C39" s="66"/>
+      <c r="D39" s="66"/>
+      <c r="E39" s="66"/>
+      <c r="F39" s="66"/>
+      <c r="G39" s="66"/>
+      <c r="H39" s="66"/>
+      <c r="I39" s="66"/>
+      <c r="J39" s="66"/>
+      <c r="K39" s="66"/>
+      <c r="L39" s="66"/>
+      <c r="M39" s="66"/>
+      <c r="N39" s="66"/>
+      <c r="O39" s="66"/>
+      <c r="P39" s="66"/>
       <c r="Q39" s="16"/>
     </row>
   </sheetData>
@@ -3104,8 +3181,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7A2A574-CCE1-411A-AF42-0ACA90961AAE}">
   <dimension ref="A1:T95"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3119,7 +3196,9 @@
     <col min="9" max="9" width="16.7109375" customWidth="1"/>
     <col min="10" max="10" width="42.5703125" customWidth="1"/>
     <col min="11" max="11" width="46.7109375" customWidth="1"/>
-    <col min="15" max="15" width="9.140625" customWidth="1"/>
+    <col min="14" max="14" width="28.85546875" customWidth="1"/>
+    <col min="15" max="15" width="80.85546875" customWidth="1"/>
+    <col min="16" max="16" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
@@ -3160,26 +3239,35 @@
       <c r="M1" s="50" t="s">
         <v>76</v>
       </c>
+      <c r="N1" s="45" t="s">
+        <v>120</v>
+      </c>
+      <c r="O1" s="45" t="s">
+        <v>121</v>
+      </c>
+      <c r="P1" s="45" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="2" spans="1:20" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="56" t="s">
+      <c r="A2" s="52" t="s">
         <v>60</v>
       </c>
-      <c r="B2" s="57" t="s">
+      <c r="B2" s="53" t="s">
         <v>81</v>
       </c>
-      <c r="C2" s="57" t="s">
+      <c r="C2" s="53" t="s">
         <v>81</v>
       </c>
-      <c r="D2" s="57" t="s">
+      <c r="D2" s="53" t="s">
         <v>81</v>
       </c>
-      <c r="E2" s="58"/>
-      <c r="F2" s="47" t="s">
-        <v>98</v>
-      </c>
-      <c r="G2" s="47" t="s">
-        <v>95</v>
+      <c r="E2" s="54"/>
+      <c r="F2" s="64" t="s">
+        <v>96</v>
+      </c>
+      <c r="G2" s="64" t="s">
+        <v>119</v>
       </c>
       <c r="H2" s="49"/>
       <c r="I2" s="41" t="str">
@@ -3196,32 +3284,34 @@
         <v>2020</v>
       </c>
       <c r="M2" s="51"/>
-      <c r="N2" s="1"/>
-      <c r="O2" s="1"/>
-      <c r="P2" s="1"/>
+      <c r="N2" s="52" t="s">
+        <v>127</v>
+      </c>
+      <c r="O2" s="42"/>
+      <c r="P2" s="64"/>
       <c r="Q2" s="1"/>
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
     </row>
     <row r="3" spans="1:20" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="59" t="s">
+      <c r="A3" s="55" t="s">
         <v>64</v>
       </c>
-      <c r="B3" s="60" t="s">
+      <c r="B3" s="56" t="s">
         <v>81</v>
       </c>
-      <c r="C3" s="60" t="s">
+      <c r="C3" s="56" t="s">
         <v>81</v>
       </c>
-      <c r="D3" s="57" t="s">
+      <c r="D3" s="56" t="s">
         <v>81</v>
       </c>
-      <c r="E3" s="58"/>
-      <c r="F3" s="48" t="s">
-        <v>97</v>
-      </c>
-      <c r="G3" s="48" t="s">
+      <c r="E3" s="54"/>
+      <c r="F3" s="65" t="s">
+        <v>95</v>
+      </c>
+      <c r="G3" s="65" t="s">
         <v>80</v>
       </c>
       <c r="H3" s="49"/>
@@ -3239,33 +3329,37 @@
         <v>2016</v>
       </c>
       <c r="M3" s="51"/>
-      <c r="N3" s="1"/>
-      <c r="O3" s="1"/>
-      <c r="P3" s="1"/>
+      <c r="N3" s="59" t="s">
+        <v>128</v>
+      </c>
+      <c r="O3" s="59" t="s">
+        <v>129</v>
+      </c>
+      <c r="P3" s="59"/>
       <c r="Q3" s="1"/>
       <c r="R3" s="1"/>
       <c r="S3" s="1"/>
       <c r="T3" s="1"/>
     </row>
     <row r="4" spans="1:20" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="56" t="s">
+      <c r="A4" s="52" t="s">
         <v>65</v>
       </c>
-      <c r="B4" s="57" t="s">
+      <c r="B4" s="53" t="s">
         <v>81</v>
       </c>
-      <c r="C4" s="57" t="s">
+      <c r="C4" s="53" t="s">
         <v>81</v>
       </c>
-      <c r="D4" s="58"/>
-      <c r="E4" s="57" t="s">
+      <c r="D4" s="54"/>
+      <c r="E4" s="53" t="s">
         <v>81</v>
       </c>
-      <c r="F4" s="47" t="s">
-        <v>98</v>
-      </c>
-      <c r="G4" s="47" t="s">
-        <v>99</v>
+      <c r="F4" s="64" t="s">
+        <v>96</v>
+      </c>
+      <c r="G4" s="64" t="s">
+        <v>97</v>
       </c>
       <c r="H4" s="49"/>
       <c r="I4" s="41" t="str">
@@ -3273,7 +3367,7 @@
         <v>[3]</v>
       </c>
       <c r="J4" s="42" t="s">
-        <v>83</v>
+        <v>117</v>
       </c>
       <c r="K4" s="3" t="s">
         <v>79</v>
@@ -3282,30 +3376,32 @@
         <v>2007</v>
       </c>
       <c r="M4" s="51"/>
-      <c r="N4" s="1"/>
-      <c r="O4" s="1"/>
-      <c r="P4" s="1"/>
+      <c r="N4" s="52" t="s">
+        <v>64</v>
+      </c>
+      <c r="O4" s="42"/>
+      <c r="P4" s="64"/>
       <c r="Q4" s="1"/>
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
       <c r="T4" s="1"/>
     </row>
     <row r="5" spans="1:20" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="59" t="s">
+      <c r="A5" s="55" t="s">
         <v>68</v>
       </c>
-      <c r="B5" s="60" t="s">
+      <c r="B5" s="56" t="s">
         <v>81</v>
       </c>
-      <c r="C5" s="60" t="s">
+      <c r="C5" s="54" t="s">
         <v>81</v>
       </c>
-      <c r="D5" s="60" t="s">
+      <c r="D5" s="56" t="s">
         <v>81</v>
       </c>
-      <c r="E5" s="58"/>
+      <c r="E5" s="54"/>
       <c r="F5" s="46" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G5" s="44"/>
       <c r="H5" s="49"/>
@@ -3314,41 +3410,43 @@
         <v>[4]</v>
       </c>
       <c r="J5" s="40" t="s">
+        <v>83</v>
+      </c>
+      <c r="K5" s="2" t="s">
         <v>84</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>85</v>
       </c>
       <c r="L5" s="40">
         <v>2014</v>
       </c>
       <c r="M5" s="51"/>
-      <c r="N5" s="1"/>
-      <c r="O5" s="1"/>
-      <c r="P5" s="1"/>
+      <c r="N5" s="71" t="s">
+        <v>65</v>
+      </c>
+      <c r="O5" s="44"/>
+      <c r="P5" s="65"/>
       <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
       <c r="T5" s="1"/>
     </row>
     <row r="6" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="56" t="s">
+      <c r="A6" s="52" t="s">
         <v>69</v>
       </c>
-      <c r="B6" s="57" t="s">
+      <c r="B6" s="53" t="s">
         <v>81</v>
       </c>
-      <c r="C6" s="57" t="s">
+      <c r="C6" s="54" t="s">
         <v>81</v>
       </c>
-      <c r="D6" s="58"/>
-      <c r="E6" s="57" t="s">
+      <c r="D6" s="54"/>
+      <c r="E6" s="53" t="s">
         <v>81</v>
       </c>
-      <c r="F6" s="47" t="s">
-        <v>98</v>
-      </c>
-      <c r="G6" s="61"/>
+      <c r="F6" s="64" t="s">
+        <v>96</v>
+      </c>
+      <c r="G6" s="57"/>
       <c r="H6" s="49"/>
       <c r="I6" s="47" t="str">
         <f>HYPERLINK("https://medium.com/athena-talks/my-first-virtual-reality-sexual-assault-2330410b62ee  ", "[5]")</f>
@@ -3358,34 +3456,36 @@
         <v>60</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="L6" s="42">
         <v>2016</v>
       </c>
       <c r="M6" s="51"/>
-      <c r="N6" s="1"/>
-      <c r="O6" s="1"/>
-      <c r="P6" s="1"/>
+      <c r="N6" s="52" t="s">
+        <v>68</v>
+      </c>
+      <c r="O6" s="42"/>
+      <c r="P6" s="64"/>
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
       <c r="S6" s="1"/>
       <c r="T6" s="1"/>
     </row>
     <row r="7" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="59" t="s">
-        <v>86</v>
-      </c>
-      <c r="B7" s="60" t="s">
+      <c r="A7" s="55" t="s">
+        <v>85</v>
+      </c>
+      <c r="B7" s="56" t="s">
         <v>81</v>
       </c>
-      <c r="C7" s="60" t="s">
+      <c r="C7" s="54" t="s">
         <v>81</v>
       </c>
-      <c r="D7" s="60" t="s">
+      <c r="D7" s="56" t="s">
         <v>81</v>
       </c>
-      <c r="E7" s="58"/>
+      <c r="E7" s="54"/>
       <c r="F7" s="46" t="str">
         <f>HYPERLINK("https://drulibrary.uoregon.edu/sites/drulibrary2.uoregon.edu/files/rpds/entry/file_for_download/National_Street_Harassment_Report.pdf  ", "[4]")</f>
         <v>[4]</v>
@@ -3400,38 +3500,40 @@
         <v>64</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="L7" s="40">
         <v>2013</v>
       </c>
       <c r="M7" s="51"/>
-      <c r="N7" s="1"/>
-      <c r="O7" s="1"/>
-      <c r="P7" s="1"/>
+      <c r="N7" s="71" t="s">
+        <v>69</v>
+      </c>
+      <c r="O7" s="44"/>
+      <c r="P7" s="65"/>
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
       <c r="S7" s="1"/>
       <c r="T7" s="1"/>
     </row>
-    <row r="8" spans="1:20" ht="63" x14ac:dyDescent="0.25">
-      <c r="A8" s="56" t="s">
-        <v>102</v>
-      </c>
-      <c r="B8" s="57" t="s">
+    <row r="8" spans="1:20" ht="63.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="52" t="s">
+        <v>100</v>
+      </c>
+      <c r="B8" s="53" t="s">
         <v>81</v>
       </c>
-      <c r="C8" s="57" t="s">
+      <c r="C8" s="54" t="s">
         <v>81</v>
       </c>
-      <c r="D8" s="57" t="s">
+      <c r="D8" s="53" t="s">
         <v>81</v>
       </c>
-      <c r="E8" s="58"/>
-      <c r="F8" s="47" t="s">
-        <v>100</v>
-      </c>
-      <c r="G8" s="62"/>
+      <c r="E8" s="54"/>
+      <c r="F8" s="64" t="s">
+        <v>98</v>
+      </c>
+      <c r="G8" s="58"/>
       <c r="H8" s="49"/>
       <c r="I8" s="47" t="str">
         <f>HYPERLINK("https://dl.acm.org/doi/abs/10.1145/3359202?casa_token=0NUecOTYG_YAAAAA:KvTubl6e8UnX8572gKMhU3ZCVQD5PPTJlPIb7DozmmEI2DNB2on9cf2V2y-QS7ruccgIDan_Us-_2w%22  ", "[7]")</f>
@@ -3447,195 +3549,205 @@
         <v>2019</v>
       </c>
       <c r="M8" s="51"/>
-      <c r="N8" s="1"/>
-      <c r="O8" s="1"/>
-      <c r="P8" s="1"/>
+      <c r="N8" s="52" t="s">
+        <v>85</v>
+      </c>
+      <c r="O8" s="42"/>
+      <c r="P8" s="64"/>
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
       <c r="S8" s="1"/>
       <c r="T8" s="1"/>
     </row>
-    <row r="9" spans="1:20" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="59" t="s">
-        <v>87</v>
-      </c>
-      <c r="B9" s="60" t="s">
+    <row r="9" spans="1:20" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A9" s="55" t="s">
+        <v>86</v>
+      </c>
+      <c r="B9" s="56" t="s">
         <v>81</v>
       </c>
-      <c r="C9" s="60" t="s">
+      <c r="C9" s="54" t="s">
         <v>81</v>
       </c>
-      <c r="D9" s="58"/>
-      <c r="E9" s="60" t="s">
+      <c r="D9" s="54"/>
+      <c r="E9" s="56" t="s">
         <v>81</v>
       </c>
-      <c r="F9" s="46" t="s">
-        <v>104</v>
-      </c>
-      <c r="G9" s="63"/>
+      <c r="F9" s="63" t="s">
+        <v>102</v>
+      </c>
+      <c r="G9" s="59"/>
       <c r="H9" s="49"/>
       <c r="I9" s="46" t="str">
         <f>HYPERLINK("https://www.emerald.com/insight/content/doi/10.1108/JCRPP-08-2016-0016/full/pdf?title=the-prevalence-and-nature-of-sexual-harassment-and-assault-against-women-and-girls-on-public-transport-an-international-review", "[8]")</f>
         <v>[8]</v>
       </c>
       <c r="J9" s="40" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="L9" s="40">
         <v>2016</v>
       </c>
       <c r="M9" s="51"/>
-      <c r="N9" s="1"/>
-      <c r="O9" s="1"/>
-      <c r="P9" s="1"/>
+      <c r="N9" s="71" t="s">
+        <v>100</v>
+      </c>
+      <c r="O9" s="44"/>
+      <c r="P9" s="65"/>
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
       <c r="S9" s="1"/>
       <c r="T9" s="1"/>
     </row>
     <row r="10" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="56" t="s">
-        <v>88</v>
-      </c>
-      <c r="B10" s="57" t="s">
+      <c r="A10" s="52" t="s">
+        <v>87</v>
+      </c>
+      <c r="B10" s="53" t="s">
         <v>81</v>
       </c>
-      <c r="C10" s="57" t="s">
+      <c r="C10" s="54" t="s">
         <v>81</v>
       </c>
-      <c r="D10" s="64" t="s">
+      <c r="D10" s="60" t="s">
         <v>81</v>
       </c>
-      <c r="E10" s="57" t="s">
+      <c r="E10" s="53" t="s">
         <v>81</v>
       </c>
-      <c r="F10" s="47" t="s">
-        <v>100</v>
-      </c>
-      <c r="G10" s="62"/>
+      <c r="F10" s="64" t="s">
+        <v>98</v>
+      </c>
+      <c r="G10" s="58"/>
       <c r="H10" s="49"/>
       <c r="I10" s="47" t="str">
         <f>HYPERLINK("https://www.sciencedirect.com/science/article/pii/S0733862705700912?ref=pdf_download&amp;fr=RR-2&amp;rr=86e94c45fdb26b52  ", "[9]")</f>
         <v>[9]</v>
       </c>
       <c r="J10" s="42" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="L10" s="42">
         <v>1999</v>
       </c>
       <c r="M10" s="51"/>
-      <c r="N10" s="1"/>
-      <c r="O10" s="1"/>
-      <c r="P10" s="1"/>
+      <c r="N10" s="52" t="s">
+        <v>86</v>
+      </c>
+      <c r="O10" s="42"/>
+      <c r="P10" s="64"/>
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
       <c r="S10" s="1"/>
       <c r="T10" s="1"/>
     </row>
     <row r="11" spans="1:20" ht="45" x14ac:dyDescent="0.25">
-      <c r="A11" s="59" t="s">
-        <v>89</v>
-      </c>
-      <c r="B11" s="60" t="s">
+      <c r="A11" s="55" t="s">
+        <v>88</v>
+      </c>
+      <c r="B11" s="56" t="s">
         <v>81</v>
       </c>
-      <c r="C11" s="60" t="s">
+      <c r="C11" s="54" t="s">
         <v>81</v>
       </c>
-      <c r="D11" s="58"/>
-      <c r="E11" s="60" t="s">
+      <c r="D11" s="54"/>
+      <c r="E11" s="56" t="s">
         <v>81</v>
       </c>
-      <c r="F11" s="63"/>
-      <c r="G11" s="63"/>
+      <c r="F11" s="59"/>
+      <c r="G11" s="59"/>
       <c r="H11" s="49"/>
       <c r="I11" s="46" t="str">
         <f>HYPERLINK("https://pubmed.ncbi.nlm.nih.gov/23813664/  ", "[10]")</f>
         <v>[10]</v>
       </c>
       <c r="J11" s="40" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="L11" s="40">
         <v>2013</v>
       </c>
       <c r="M11" s="51"/>
-      <c r="N11" s="1"/>
-      <c r="O11" s="1"/>
-      <c r="P11" s="1"/>
+      <c r="N11" s="71" t="s">
+        <v>87</v>
+      </c>
+      <c r="O11" s="44"/>
+      <c r="P11" s="65"/>
       <c r="Q11" s="1"/>
       <c r="R11" s="1"/>
       <c r="S11" s="1"/>
       <c r="T11" s="1"/>
     </row>
     <row r="12" spans="1:20" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="56" t="s">
-        <v>90</v>
-      </c>
-      <c r="B12" s="57" t="s">
+      <c r="A12" s="52" t="s">
+        <v>89</v>
+      </c>
+      <c r="B12" s="53" t="s">
         <v>81</v>
       </c>
-      <c r="C12" s="57" t="s">
+      <c r="C12" s="54" t="s">
         <v>81</v>
       </c>
-      <c r="D12" s="58"/>
-      <c r="E12" s="57" t="s">
+      <c r="D12" s="54"/>
+      <c r="E12" s="53" t="s">
         <v>81</v>
       </c>
-      <c r="F12" s="47" t="s">
-        <v>106</v>
-      </c>
-      <c r="G12" s="62"/>
+      <c r="F12" s="64" t="s">
+        <v>104</v>
+      </c>
+      <c r="G12" s="58"/>
       <c r="H12" s="49"/>
       <c r="I12" s="47" t="str">
         <f>HYPERLINK("https://www.mic.com/articles/144470/sexual-harassment-in-virtual-reality  ", "[11]")</f>
         <v>[11]</v>
       </c>
       <c r="J12" s="42" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="L12" s="42">
         <v>2016</v>
       </c>
       <c r="M12" s="51"/>
-      <c r="N12" s="1"/>
-      <c r="O12" s="1"/>
-      <c r="P12" s="1"/>
+      <c r="N12" s="52" t="s">
+        <v>88</v>
+      </c>
+      <c r="O12" s="42"/>
+      <c r="P12" s="64"/>
       <c r="Q12" s="1"/>
       <c r="R12" s="1"/>
       <c r="S12" s="1"/>
       <c r="T12" s="1"/>
     </row>
     <row r="13" spans="1:20" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="59" t="s">
-        <v>91</v>
-      </c>
-      <c r="B13" s="65" t="s">
+      <c r="A13" s="55" t="s">
+        <v>90</v>
+      </c>
+      <c r="B13" s="61" t="s">
         <v>81</v>
       </c>
-      <c r="C13" s="60" t="s">
+      <c r="C13" s="56" t="s">
         <v>81</v>
       </c>
-      <c r="D13" s="60" t="s">
+      <c r="D13" s="56" t="s">
         <v>81</v>
       </c>
-      <c r="E13" s="58"/>
-      <c r="F13" s="63"/>
-      <c r="G13" s="46" t="s">
-        <v>109</v>
+      <c r="E13" s="54"/>
+      <c r="F13" s="59"/>
+      <c r="G13" s="63" t="s">
+        <v>107</v>
       </c>
       <c r="H13" s="49"/>
       <c r="I13" s="48" t="str">
@@ -3643,40 +3755,42 @@
         <v>[12]</v>
       </c>
       <c r="J13" s="40" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="L13" s="40">
         <v>2022</v>
       </c>
       <c r="M13" s="51"/>
-      <c r="N13" s="1"/>
-      <c r="O13" s="1"/>
-      <c r="P13" s="1"/>
+      <c r="N13" s="71" t="s">
+        <v>89</v>
+      </c>
+      <c r="O13" s="44"/>
+      <c r="P13" s="65"/>
       <c r="Q13" s="1"/>
       <c r="R13" s="1"/>
       <c r="S13" s="1"/>
       <c r="T13" s="1"/>
     </row>
     <row r="14" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="56" t="s">
-        <v>92</v>
-      </c>
-      <c r="B14" s="57" t="s">
+      <c r="A14" s="52" t="s">
+        <v>91</v>
+      </c>
+      <c r="B14" s="53" t="s">
         <v>81</v>
       </c>
-      <c r="C14" s="66" t="s">
+      <c r="C14" s="62" t="s">
         <v>81</v>
       </c>
-      <c r="D14" s="58"/>
-      <c r="E14" s="57" t="s">
+      <c r="D14" s="54"/>
+      <c r="E14" s="53" t="s">
         <v>81</v>
       </c>
-      <c r="F14" s="62"/>
-      <c r="G14" s="47" t="s">
-        <v>110</v>
+      <c r="F14" s="58"/>
+      <c r="G14" s="64" t="s">
+        <v>108</v>
       </c>
       <c r="H14" s="49"/>
       <c r="I14" s="47" t="str">
@@ -3684,37 +3798,39 @@
         <v>[13]</v>
       </c>
       <c r="J14" s="42" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="L14" s="42">
         <v>2020</v>
       </c>
       <c r="M14" s="51"/>
-      <c r="N14" s="1"/>
-      <c r="O14" s="1"/>
-      <c r="P14" s="1"/>
+      <c r="N14" s="52" t="s">
+        <v>90</v>
+      </c>
+      <c r="O14" s="42"/>
+      <c r="P14" s="64"/>
       <c r="Q14" s="1"/>
       <c r="R14" s="1"/>
       <c r="S14" s="1"/>
       <c r="T14" s="1"/>
     </row>
     <row r="15" spans="1:20" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="59" t="s">
-        <v>111</v>
-      </c>
-      <c r="B15" s="58"/>
-      <c r="C15" s="60" t="s">
+      <c r="A15" s="55" t="s">
+        <v>109</v>
+      </c>
+      <c r="B15" s="54"/>
+      <c r="C15" s="56" t="s">
         <v>81</v>
       </c>
-      <c r="D15" s="58"/>
-      <c r="E15" s="60" t="s">
+      <c r="D15" s="54"/>
+      <c r="E15" s="56" t="s">
         <v>81</v>
       </c>
-      <c r="F15" s="46" t="s">
-        <v>112</v>
+      <c r="F15" s="63" t="s">
+        <v>110</v>
       </c>
       <c r="G15" s="46"/>
       <c r="H15" s="49"/>
@@ -3723,38 +3839,40 @@
         <v>[14]</v>
       </c>
       <c r="J15" s="40" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="L15" s="40">
         <v>2024</v>
       </c>
       <c r="M15" s="51"/>
-      <c r="N15" s="1"/>
-      <c r="O15" s="1"/>
-      <c r="P15" s="1"/>
+      <c r="N15" s="71" t="s">
+        <v>91</v>
+      </c>
+      <c r="O15" s="44"/>
+      <c r="P15" s="65"/>
       <c r="Q15" s="1"/>
       <c r="R15" s="1"/>
       <c r="S15" s="1"/>
       <c r="T15" s="1"/>
     </row>
     <row r="16" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="56" t="s">
-        <v>93</v>
-      </c>
-      <c r="B16" s="58"/>
-      <c r="C16" s="57" t="s">
+      <c r="A16" s="52" t="s">
+        <v>92</v>
+      </c>
+      <c r="B16" s="54"/>
+      <c r="C16" s="53" t="s">
         <v>81</v>
       </c>
-      <c r="D16" s="57" t="s">
+      <c r="D16" s="53" t="s">
         <v>81</v>
       </c>
-      <c r="E16" s="58"/>
-      <c r="F16" s="62"/>
-      <c r="G16" s="47" t="s">
-        <v>113</v>
+      <c r="E16" s="54"/>
+      <c r="F16" s="58"/>
+      <c r="G16" s="64" t="s">
+        <v>111</v>
       </c>
       <c r="H16" s="49"/>
       <c r="I16" s="47" t="str">
@@ -3762,110 +3880,124 @@
         <v>[15]</v>
       </c>
       <c r="J16" s="42" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="L16" s="42">
         <v>2020</v>
       </c>
       <c r="M16" s="51"/>
-      <c r="N16" s="1"/>
-      <c r="O16" s="1"/>
-      <c r="P16" s="1"/>
+      <c r="N16" s="52" t="s">
+        <v>109</v>
+      </c>
+      <c r="O16" s="42"/>
+      <c r="P16" s="64"/>
       <c r="Q16" s="1"/>
       <c r="R16" s="1"/>
       <c r="S16" s="1"/>
       <c r="T16" s="1"/>
     </row>
     <row r="17" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" s="59" t="s">
-        <v>115</v>
-      </c>
-      <c r="B17" s="60" t="s">
+      <c r="A17" s="55" t="s">
+        <v>113</v>
+      </c>
+      <c r="B17" s="56" t="s">
         <v>81</v>
       </c>
-      <c r="C17" s="60" t="s">
+      <c r="C17" s="56" t="s">
         <v>81</v>
       </c>
-      <c r="D17" s="58"/>
-      <c r="E17" s="60" t="s">
+      <c r="D17" s="54"/>
+      <c r="E17" s="56" t="s">
         <v>81</v>
       </c>
-      <c r="F17" s="46">
-        <v>15</v>
-      </c>
-      <c r="G17" s="63"/>
+      <c r="F17" s="63" t="s">
+        <v>118</v>
+      </c>
+      <c r="G17" s="59"/>
       <c r="H17" s="49"/>
       <c r="I17" s="40"/>
       <c r="J17" s="40"/>
       <c r="K17" s="2"/>
       <c r="L17" s="40"/>
       <c r="M17" s="51"/>
-      <c r="N17" s="1"/>
-      <c r="O17" s="1"/>
-      <c r="P17" s="1"/>
+      <c r="N17" s="71" t="s">
+        <v>92</v>
+      </c>
+      <c r="O17" s="44"/>
+      <c r="P17" s="65"/>
       <c r="Q17" s="1"/>
       <c r="R17" s="1"/>
       <c r="S17" s="1"/>
       <c r="T17" s="1"/>
     </row>
     <row r="18" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" s="59" t="s">
-        <v>118</v>
-      </c>
-      <c r="B18" s="57" t="s">
+      <c r="A18" s="52" t="s">
+        <v>116</v>
+      </c>
+      <c r="B18" s="53" t="s">
         <v>81</v>
       </c>
-      <c r="C18" s="57" t="s">
+      <c r="C18" s="53" t="s">
         <v>81</v>
       </c>
-      <c r="D18" s="58"/>
-      <c r="E18" s="57" t="s">
+      <c r="D18" s="54"/>
+      <c r="E18" s="53" t="s">
         <v>81</v>
       </c>
-      <c r="F18" s="46">
-        <v>16</v>
-      </c>
-      <c r="G18" s="67"/>
+      <c r="F18" s="47"/>
+      <c r="G18" s="70"/>
       <c r="H18" s="49"/>
       <c r="I18" s="42"/>
       <c r="J18" s="42"/>
       <c r="K18" s="3"/>
       <c r="L18" s="42"/>
       <c r="M18" s="51"/>
-      <c r="N18" s="1"/>
-      <c r="O18" s="1"/>
-      <c r="P18" s="1"/>
+      <c r="N18" s="52" t="s">
+        <v>113</v>
+      </c>
+      <c r="O18" s="42"/>
+      <c r="P18" s="64"/>
       <c r="Q18" s="1"/>
       <c r="R18" s="1"/>
       <c r="S18" s="1"/>
       <c r="T18" s="1"/>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.25">
-      <c r="A19" s="49"/>
-      <c r="B19" s="49"/>
-      <c r="C19" s="49"/>
-      <c r="D19" s="49"/>
-      <c r="E19" s="49"/>
-      <c r="F19" s="49"/>
-      <c r="G19" s="49"/>
+    <row r="19" spans="1:20" ht="63" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="71" t="s">
+        <v>122</v>
+      </c>
+      <c r="B19" s="54" t="s">
+        <v>81</v>
+      </c>
+      <c r="C19" s="56" t="s">
+        <v>81</v>
+      </c>
+      <c r="D19" s="54"/>
+      <c r="E19" s="54"/>
+      <c r="F19" s="48"/>
+      <c r="G19" s="65" t="s">
+        <v>124</v>
+      </c>
       <c r="H19" s="49"/>
       <c r="I19" s="40"/>
       <c r="J19" s="40"/>
       <c r="K19" s="2"/>
       <c r="L19" s="40"/>
       <c r="M19" s="51"/>
-      <c r="N19" s="1"/>
-      <c r="O19" s="1"/>
-      <c r="P19" s="1"/>
+      <c r="N19" s="71" t="s">
+        <v>116</v>
+      </c>
+      <c r="O19" s="44"/>
+      <c r="P19" s="65"/>
       <c r="Q19" s="1"/>
       <c r="R19" s="1"/>
       <c r="S19" s="1"/>
       <c r="T19" s="1"/>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:20" ht="60" x14ac:dyDescent="0.25">
       <c r="A20" s="49"/>
       <c r="B20" s="49"/>
       <c r="C20" s="49"/>
@@ -3879,15 +4011,21 @@
       <c r="K20" s="3"/>
       <c r="L20" s="42"/>
       <c r="M20" s="51"/>
-      <c r="N20" s="1"/>
-      <c r="O20" s="1"/>
-      <c r="P20" s="1"/>
+      <c r="N20" s="52" t="s">
+        <v>122</v>
+      </c>
+      <c r="O20" s="42" t="s">
+        <v>123</v>
+      </c>
+      <c r="P20" s="64" t="s">
+        <v>124</v>
+      </c>
       <c r="Q20" s="1"/>
       <c r="R20" s="1"/>
       <c r="S20" s="1"/>
       <c r="T20" s="1"/>
     </row>
-    <row r="21" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="49"/>
       <c r="B21" s="49"/>
       <c r="C21" s="49"/>
@@ -3901,15 +4039,15 @@
       <c r="K21" s="2"/>
       <c r="L21" s="40"/>
       <c r="M21" s="51"/>
-      <c r="N21" s="1"/>
-      <c r="O21" s="1"/>
-      <c r="P21" s="1"/>
+      <c r="N21" s="71"/>
+      <c r="O21" s="44"/>
+      <c r="P21" s="65"/>
       <c r="Q21" s="1"/>
       <c r="R21" s="1"/>
       <c r="S21" s="1"/>
       <c r="T21" s="1"/>
     </row>
-    <row r="22" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="49"/>
       <c r="B22" s="49"/>
       <c r="C22" s="49"/>
@@ -3923,15 +4061,15 @@
       <c r="K22" s="3"/>
       <c r="L22" s="42"/>
       <c r="M22" s="51"/>
-      <c r="N22" s="1"/>
-      <c r="O22" s="1"/>
-      <c r="P22" s="1"/>
+      <c r="N22" s="52"/>
+      <c r="O22" s="42"/>
+      <c r="P22" s="64"/>
       <c r="Q22" s="1"/>
       <c r="R22" s="1"/>
       <c r="S22" s="1"/>
       <c r="T22" s="1"/>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="49"/>
       <c r="B23" s="49"/>
       <c r="C23" s="49"/>
@@ -3945,15 +4083,15 @@
       <c r="K23" s="2"/>
       <c r="L23" s="40"/>
       <c r="M23" s="51"/>
-      <c r="N23" s="1"/>
-      <c r="O23" s="1"/>
-      <c r="P23" s="1"/>
+      <c r="N23" s="71"/>
+      <c r="O23" s="44"/>
+      <c r="P23" s="65"/>
       <c r="Q23" s="1"/>
       <c r="R23" s="1"/>
       <c r="S23" s="1"/>
       <c r="T23" s="1"/>
     </row>
-    <row r="24" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="49"/>
       <c r="B24" s="49"/>
       <c r="C24" s="49"/>
@@ -3967,15 +4105,15 @@
       <c r="K24" s="3"/>
       <c r="L24" s="42"/>
       <c r="M24" s="51"/>
-      <c r="N24" s="1"/>
-      <c r="O24" s="1"/>
-      <c r="P24" s="1"/>
+      <c r="N24" s="52"/>
+      <c r="O24" s="42"/>
+      <c r="P24" s="64"/>
       <c r="Q24" s="1"/>
       <c r="R24" s="1"/>
       <c r="S24" s="1"/>
       <c r="T24" s="1"/>
     </row>
-    <row r="25" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="49"/>
       <c r="B25" s="49"/>
       <c r="C25" s="49"/>
@@ -3989,15 +4127,15 @@
       <c r="K25" s="2"/>
       <c r="L25" s="40"/>
       <c r="M25" s="51"/>
-      <c r="N25" s="1"/>
-      <c r="O25" s="1"/>
-      <c r="P25" s="1"/>
+      <c r="N25" s="71"/>
+      <c r="O25" s="44"/>
+      <c r="P25" s="65"/>
       <c r="Q25" s="1"/>
       <c r="R25" s="1"/>
       <c r="S25" s="1"/>
       <c r="T25" s="1"/>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="49"/>
       <c r="B26" s="49"/>
       <c r="C26" s="49"/>
@@ -4011,15 +4149,15 @@
       <c r="K26" s="3"/>
       <c r="L26" s="42"/>
       <c r="M26" s="51"/>
-      <c r="N26" s="1"/>
-      <c r="O26" s="1"/>
-      <c r="P26" s="1"/>
+      <c r="N26" s="52"/>
+      <c r="O26" s="42"/>
+      <c r="P26" s="64"/>
       <c r="Q26" s="1"/>
       <c r="R26" s="1"/>
       <c r="S26" s="1"/>
       <c r="T26" s="1"/>
     </row>
-    <row r="27" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="49"/>
       <c r="B27" s="49"/>
       <c r="C27" s="49"/>
@@ -4033,15 +4171,15 @@
       <c r="K27" s="2"/>
       <c r="L27" s="40"/>
       <c r="M27" s="51"/>
-      <c r="N27" s="1"/>
-      <c r="O27" s="1"/>
-      <c r="P27" s="1"/>
+      <c r="N27" s="71"/>
+      <c r="O27" s="44"/>
+      <c r="P27" s="65"/>
       <c r="Q27" s="1"/>
       <c r="R27" s="1"/>
       <c r="S27" s="1"/>
       <c r="T27" s="1"/>
     </row>
-    <row r="28" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A28" s="49"/>
       <c r="B28" s="49"/>
       <c r="C28" s="49"/>
@@ -4055,9 +4193,9 @@
       <c r="K28" s="3"/>
       <c r="L28" s="42"/>
       <c r="M28" s="51"/>
-      <c r="N28" s="1"/>
-      <c r="O28" s="1"/>
-      <c r="P28" s="1"/>
+      <c r="N28" s="52"/>
+      <c r="O28" s="42"/>
+      <c r="P28" s="64"/>
       <c r="Q28" s="1"/>
       <c r="R28" s="1"/>
       <c r="S28" s="1"/>

</xml_diff>